<commit_message>
All currencies markets refresh
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_Market.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="206">
   <si>
     <t>PriceTickValue</t>
   </si>
@@ -700,6 +700,9 @@
   </si>
   <si>
     <t>HkdHibor6M</t>
+  </si>
+  <si>
+    <t>Record not service permissioned</t>
   </si>
 </sst>
 </file>
@@ -2199,75 +2202,65 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
         <stp/>
-        <stp>{9BF9BAEB-0C1E-47B8-973D-DF4F5BBC07F1}</stp>
-        <tr r="L4" s="17"/>
+        <stp>{D116319A-9970-40B0-9A4A-974B6850C4F2}</stp>
+        <tr r="M4" s="10"/>
       </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
         <stp/>
-        <stp>{8552C64A-82B9-40E8-82C6-4D8C83A4BEBD}</stp>
+        <stp>{C9DCCDCA-05F4-4CA9-A0F8-BC01AB9C3430}</stp>
+        <tr r="T5" s="36"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:38:24</v>
+        <stp/>
+        <stp>{E2A452ED-0103-4632-BD55-FB44213EC468}</stp>
+        <tr r="O3" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:38:20</v>
+        <stp/>
+        <stp>{8DC5C32F-6A5E-4831-85F2-DE89AC5CF822}</stp>
         <tr r="I3" s="9"/>
       </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
         <stp/>
-        <stp>{FB0A55E0-EACB-4562-A7E2-889319234D2D}</stp>
+        <stp>{98427C89-F10D-4F48-9C37-9A1E7C8AB197}</stp>
         <tr r="L4" s="19"/>
       </tp>
       <tp t="s">
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
         <stp/>
-        <stp>{787D5198-4821-4342-9F37-A537DB97E67F}</stp>
-        <tr r="O3" s="12"/>
-      </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 10:23:59</v>
-        <stp/>
-        <stp>{4CA65FB7-9198-4F95-B578-C93079EA23F0}</stp>
-        <tr r="T5" s="36"/>
+        <stp>{13E4E301-94B3-4F3E-BCFD-034A2BD02025}</stp>
+        <tr r="L4" s="17"/>
       </tp>
       <tp t="s">
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
         <stp/>
-        <stp>{7185F528-0F02-43DD-840C-7D1BDF37CF4B}</stp>
-        <tr r="S4" s="5"/>
-      </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 10:23:59</v>
-        <stp/>
-        <stp>{0C972AAA-C122-49DD-BDA2-D3B9D1DA4089}</stp>
+        <stp>{6AF6A0BA-6E1D-4EFB-987E-27C976AAF5B5}</stp>
         <tr r="L4" s="16"/>
       </tp>
       <tp t="s">
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
         <stp/>
-        <stp>{91C6B259-3E5E-43ED-AD7E-54D7554388C9}</stp>
+        <stp>{C2D81708-0709-4B62-833D-7C87DED1D05E}</stp>
         <tr r="S4" s="6"/>
       </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
         <stp/>
-        <stp>{562F947C-EC14-4DFD-A42D-C98C51B1B476}</stp>
-        <tr r="M4" s="10"/>
+        <stp>{A6A2B068-96CB-45FD-B838-914DEAEC72BB}</stp>
+        <tr r="S4" s="5"/>
       </tp>
     </main>
     <main first="pldatasource.rhistoryrtdserver">
       <tp t="s">
-        <v>Updated at 10:24:00</v>
+        <v>Updated at 09:38:21</v>
         <stp/>
-        <stp>{F82BFA33-9FE3-4F1D-9DEC-32562BF26339}_x0000_</stp>
+        <stp>{19C5EE25-0BA2-403F-96F3-311FA44FCAC8}_x0000_</stp>
         <tr r="E2" s="41"/>
       </tp>
     </main>
@@ -2566,7 +2559,7 @@
   <dimension ref="B1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2581,7 +2574,7 @@
     <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="377" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Mar  3 2014 10:58:57</v>
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Apr 29 2014 14:47:17</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2604,7 +2597,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="11">
-        <v>41736.43310185185</v>
+        <v>41809.401365740741</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -2620,7 +2613,7 @@
         <v>174</v>
       </c>
       <c r="D6" s="344">
-        <v>41606.766168981485</v>
+        <v>41809.401747685188</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -2683,7 +2676,7 @@
       </c>
       <c r="D13" s="15" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Projects\quantlib\QuantLibXL\Data2\XML\</v>
+        <v>C:\Projects\quantlib.nando\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -2766,7 +2759,7 @@
       </c>
       <c r="D22" s="286">
         <f>_xll.ohTrigger(ISERROR(OIS!V3),ISERROR(Deposits!O2),ISERROR(FRA!W3),ISERROR(Futures3M!Z2),ISERROR(Swaps1M!V3),ISERROR(Swap3M!V3),ISERROR(BasisSwap1M3M!AD3),ISERROR(BasisSwap3M6M!AD3),ISERROR('Hibor Time Series'!J5:L13))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22" s="284"/>
     </row>
@@ -3074,7 +3067,7 @@
       <c r="R4" s="217"/>
       <c r="S4" s="180" t="str">
         <f>_xll.RData(S5:S42,T4:U4,,ReutersRtMode,,T5)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="T4" s="216" t="s">
         <v>160</v>
@@ -6612,7 +6605,7 @@
       <c r="AC3" s="220"/>
       <c r="AD3" s="181">
         <f>_xll.ohTrigger(AD5:AD42)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE3" s="158"/>
       <c r="AF3" s="190"/>
@@ -6652,7 +6645,7 @@
       <c r="R4" s="217"/>
       <c r="S4" s="180" t="str">
         <f>_xll.RData(S5:S42,T4:U4,,ReutersRtMode,,T5)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="T4" s="216" t="s">
         <v>160</v>
@@ -10625,7 +10618,7 @@
       </c>
       <c r="T5" s="310" t="str">
         <f>_xll.RData(T6:T14,U5:V5,"RTFEED:IDN",,,U6)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="U5" s="310" t="s">
         <v>178</v>
@@ -10705,10 +10698,10 @@
         <v>HIHKDOND=</v>
       </c>
       <c r="U6" s="308">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V6" s="337">
-        <v>5.6610000000000001E-2</v>
+        <v>6.2140000000000001E-2</v>
       </c>
       <c r="W6" s="307" t="b">
         <f t="shared" ref="W6:W14" si="2">IF(AND(ISNUMBER($V6),$V6&lt;&gt;0%),TRUE,FALSE)</f>
@@ -10720,7 +10713,7 @@
       </c>
       <c r="Y6" s="340">
         <f>_xll.qlQuoteValue(M6,X6)</f>
-        <v>5.6610000000000005E-4</v>
+        <v>6.2140000000000003E-4</v>
       </c>
       <c r="Z6" s="321"/>
     </row>
@@ -10783,10 +10776,10 @@
         <v>HIHKD1WD=</v>
       </c>
       <c r="U7" s="304">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V7" s="338">
-        <v>0.12714</v>
+        <v>0.13142999999999999</v>
       </c>
       <c r="W7" s="303" t="b">
         <f t="shared" si="2"/>
@@ -10798,7 +10791,7 @@
       </c>
       <c r="Y7" s="341">
         <f>_xll.qlQuoteValue(M7,X7)</f>
-        <v>1.2714E-3</v>
+        <v>1.3143E-3</v>
       </c>
       <c r="Z7" s="321"/>
     </row>
@@ -10863,10 +10856,10 @@
         <v>HIHKD2WD=</v>
       </c>
       <c r="U8" s="304">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V8" s="338">
-        <v>0.15643000000000001</v>
+        <v>0.16571</v>
       </c>
       <c r="W8" s="303" t="b">
         <f t="shared" si="2"/>
@@ -10878,7 +10871,7 @@
       </c>
       <c r="Y8" s="341">
         <f>_xll.qlQuoteValue(M8,X8)</f>
-        <v>1.5643000000000002E-3</v>
+        <v>1.6570999999999999E-3</v>
       </c>
       <c r="Z8" s="321"/>
     </row>
@@ -10943,10 +10936,10 @@
         <v>HIHKD1MD=</v>
       </c>
       <c r="U9" s="304">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V9" s="338">
-        <v>0.20571</v>
+        <v>0.21143000000000001</v>
       </c>
       <c r="W9" s="303" t="b">
         <f t="shared" si="2"/>
@@ -10958,7 +10951,7 @@
       </c>
       <c r="Y9" s="341">
         <f>_xll.qlQuoteValue(M9,X9)</f>
-        <v>2.0571000000000001E-3</v>
+        <v>2.1142999999999999E-3</v>
       </c>
       <c r="Z9" s="321"/>
     </row>
@@ -11023,10 +11016,10 @@
         <v>HIHKD2MD=</v>
       </c>
       <c r="U10" s="304">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V10" s="338">
-        <v>0.30286000000000002</v>
+        <v>0.29820000000000002</v>
       </c>
       <c r="W10" s="303" t="b">
         <f t="shared" si="2"/>
@@ -11038,7 +11031,7 @@
       </c>
       <c r="Y10" s="341">
         <f>_xll.qlQuoteValue(M10,X10)</f>
-        <v>3.0286000000000002E-3</v>
+        <v>2.9820000000000003E-3</v>
       </c>
       <c r="Z10" s="321"/>
     </row>
@@ -11103,10 +11096,10 @@
         <v>HIHKD3MD=</v>
       </c>
       <c r="U11" s="304">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V11" s="338">
-        <v>0.37142999999999998</v>
+        <v>0.37357000000000001</v>
       </c>
       <c r="W11" s="303" t="b">
         <f t="shared" si="2"/>
@@ -11118,7 +11111,7 @@
       </c>
       <c r="Y11" s="341">
         <f>_xll.qlQuoteValue(M11,X11)</f>
-        <v>3.7142999999999998E-3</v>
+        <v>3.7357000000000002E-3</v>
       </c>
       <c r="Z11" s="321"/>
     </row>
@@ -11183,10 +11176,10 @@
         <v>HIHKD6MD=</v>
       </c>
       <c r="U12" s="304">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V12" s="338">
-        <v>0.54857</v>
+        <v>0.54928999999999994</v>
       </c>
       <c r="W12" s="303" t="b">
         <f t="shared" si="2"/>
@@ -11198,7 +11191,7 @@
       </c>
       <c r="Y12" s="341">
         <f>_xll.qlQuoteValue(M12,X12)</f>
-        <v>5.4856999999999996E-3</v>
+        <v>5.4928999999999993E-3</v>
       </c>
       <c r="Z12" s="321"/>
     </row>
@@ -11262,23 +11255,23 @@
         <f t="shared" si="1"/>
         <v>HIHKD9MD=</v>
       </c>
-      <c r="U13" s="304">
-        <v>41729</v>
-      </c>
-      <c r="V13" s="338">
-        <v>0.64856999999999998</v>
+      <c r="U13" s="304" t="s">
+        <v>205</v>
+      </c>
+      <c r="V13" s="338" t="s">
+        <v>205</v>
       </c>
       <c r="W13" s="303" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="X13" s="302" t="b">
+        <v>0</v>
+      </c>
+      <c r="X13" s="302" t="e">
         <f>IF(W13,_xll.qlIndexAddFixings(S13,U13,V13/100,TRUE),NA())</f>
-        <v>1</v>
-      </c>
-      <c r="Y13" s="341">
+        <v>#N/A</v>
+      </c>
+      <c r="Y13" s="341" t="e">
         <f>_xll.qlQuoteValue(M13,X13)</f>
-        <v>6.4856999999999996E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="Z13" s="321"/>
     </row>
@@ -11343,10 +11336,10 @@
         <v>HIHKD1YD=</v>
       </c>
       <c r="U14" s="300">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="V14" s="339">
-        <v>0.86285999999999996</v>
+        <v>0.86356999999999995</v>
       </c>
       <c r="W14" s="299" t="b">
         <f t="shared" si="2"/>
@@ -11358,7 +11351,7 @@
       </c>
       <c r="Y14" s="342">
         <f>_xll.qlQuoteValue(M14,X14)</f>
-        <v>8.6286000000000002E-3</v>
+        <v>8.6356999999999996E-3</v>
       </c>
       <c r="Z14" s="321"/>
     </row>
@@ -11488,16 +11481,16 @@
     <row r="2" spans="1:190" s="348" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="350">
         <f>MIN(E5:E271)</f>
-        <v>41596</v>
+        <v>41799</v>
       </c>
       <c r="C2" s="350">
         <f>MAX(E5:E271)</f>
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="D2" s="351"/>
       <c r="E2" s="368" t="str">
         <f>_xll.RHistory(F2:H2,B8:C8,C3,,"CH:In;Fd TSREPEAT:N SORT:"&amp;C7,E3)</f>
-        <v>Updated at 10:24:00</v>
+        <v>Updated at 09:38:21</v>
       </c>
       <c r="F2" s="373" t="s">
         <v>200</v>
@@ -11690,7 +11683,7 @@
       </c>
       <c r="C3" s="356" t="str">
         <f>"START:"&amp;C4&amp; " END:"&amp;C5&amp;" INTERVAL:1D"</f>
-        <v>START:41726 END:41736 INTERVAL:1D</v>
+        <v>START:41799 END:41809 INTERVAL:1D</v>
       </c>
       <c r="D3" s="357"/>
       <c r="E3" s="374"/>
@@ -11719,7 +11712,7 @@
       </c>
       <c r="C4" s="360">
         <f>C5-10</f>
-        <v>41726</v>
+        <v>41799</v>
       </c>
       <c r="D4" s="357"/>
       <c r="E4" s="375" t="s">
@@ -11741,20 +11734,20 @@
       </c>
       <c r="C5" s="360">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="D5" s="357"/>
       <c r="E5" s="361">
-        <v>41736</v>
+        <v>41809</v>
       </c>
       <c r="F5" s="362">
-        <v>0.20571</v>
+        <v>0.21143000000000001</v>
       </c>
       <c r="G5" s="362">
-        <v>0.37142999999999998</v>
+        <v>0.37357000000000001</v>
       </c>
       <c r="H5" s="369">
-        <v>0.54857</v>
+        <v>0.54928999999999994</v>
       </c>
       <c r="J5" s="348" t="b">
         <f>IF(AND(ISNUMBER($E5),ISNUMBER(F5),Trigger),_xll.qlIndexAddFixings(J$3,$E5,F5/100,TRUE),NA())</f>
@@ -11772,16 +11765,16 @@
     <row r="6" spans="1:190" s="348" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D6" s="363"/>
       <c r="E6" s="361">
-        <v>41733</v>
+        <v>41808</v>
       </c>
       <c r="F6" s="362">
-        <v>0.20571</v>
+        <v>0.21429000000000001</v>
       </c>
       <c r="G6" s="362">
-        <v>0.37286000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="H6" s="369">
-        <v>0.54786000000000001</v>
+        <v>0.54847000000000001</v>
       </c>
       <c r="J6" s="348" t="b">
         <f>IF(AND(ISNUMBER($E6),ISNUMBER(F6),Trigger),_xll.qlIndexAddFixings(J$3,$E6,F6/100,TRUE),NA())</f>
@@ -11804,16 +11797,16 @@
         <v>196</v>
       </c>
       <c r="E7" s="361">
-        <v>41732</v>
+        <v>41807</v>
       </c>
       <c r="F7" s="362">
-        <v>0.20643</v>
+        <v>0.215</v>
       </c>
       <c r="G7" s="362">
-        <v>0.37357000000000001</v>
+        <v>0.37770999999999999</v>
       </c>
       <c r="H7" s="369">
-        <v>0.54928999999999994</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J7" s="348" t="b">
         <f>IF(AND(ISNUMBER($E7),ISNUMBER(F7),Trigger),_xll.qlIndexAddFixings(J$3,$E7,F7/100,TRUE),NA())</f>
@@ -11836,16 +11829,16 @@
         <v>198</v>
       </c>
       <c r="E8" s="361">
-        <v>41731</v>
+        <v>41806</v>
       </c>
       <c r="F8" s="362">
-        <v>0.20785999999999999</v>
+        <v>0.21137</v>
       </c>
       <c r="G8" s="362">
-        <v>0.37214000000000003</v>
+        <v>0.37770999999999999</v>
       </c>
       <c r="H8" s="369">
-        <v>0.54928999999999994</v>
+        <v>0.55142999999999998</v>
       </c>
       <c r="J8" s="348" t="b">
         <f>IF(AND(ISNUMBER($E8),ISNUMBER(F8),Trigger),_xll.qlIndexAddFixings(J$3,$E8,F8/100,TRUE),NA())</f>
@@ -11864,16 +11857,16 @@
       <c r="B9" s="358"/>
       <c r="C9" s="358"/>
       <c r="E9" s="361">
-        <v>41730</v>
+        <v>41803</v>
       </c>
       <c r="F9" s="362">
-        <v>0.20929</v>
+        <v>0.20910000000000001</v>
       </c>
       <c r="G9" s="362">
-        <v>0.37070999999999998</v>
+        <v>0.37429000000000001</v>
       </c>
       <c r="H9" s="369">
-        <v>0.54951000000000005</v>
+        <v>0.55071000000000003</v>
       </c>
       <c r="J9" s="348" t="b">
         <f>IF(AND(ISNUMBER($E9),ISNUMBER(F9),Trigger),_xll.qlIndexAddFixings(J$3,$E9,F9/100,TRUE),NA())</f>
@@ -11890,16 +11883,16 @@
     </row>
     <row r="10" spans="1:190" s="348" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E10" s="361">
-        <v>41729</v>
+        <v>41802</v>
       </c>
       <c r="F10" s="362">
-        <v>0.21</v>
+        <v>0.21007999999999999</v>
       </c>
       <c r="G10" s="362">
-        <v>0.37286000000000002</v>
+        <v>0.37214000000000003</v>
       </c>
       <c r="H10" s="369">
-        <v>0.55000000000000004</v>
+        <v>0.54928999999999994</v>
       </c>
       <c r="J10" s="348" t="b">
         <f>IF(AND(ISNUMBER($E10),ISNUMBER(F10),Trigger),_xll.qlIndexAddFixings(J$3,$E10,F10/100,TRUE),NA())</f>
@@ -11916,16 +11909,16 @@
     </row>
     <row r="11" spans="1:190" s="348" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E11" s="361">
-        <v>41726</v>
+        <v>41801</v>
       </c>
       <c r="F11" s="362">
-        <v>0.21</v>
+        <v>0.20643</v>
       </c>
       <c r="G11" s="362">
-        <v>0.37286000000000002</v>
+        <v>0.37134</v>
       </c>
       <c r="H11" s="369">
-        <v>0.55000000000000004</v>
+        <v>0.54857</v>
       </c>
       <c r="J11" s="348" t="b">
         <f>IF(AND(ISNUMBER($E11),ISNUMBER(F11),Trigger),_xll.qlIndexAddFixings(J$3,$E11,F11/100,TRUE),NA())</f>
@@ -11942,54 +11935,54 @@
     </row>
     <row r="12" spans="1:190" s="348" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E12" s="361">
-        <v>41597</v>
+        <v>41800</v>
       </c>
       <c r="F12" s="362">
-        <v>0.21357000000000001</v>
+        <v>0.20751</v>
       </c>
       <c r="G12" s="362">
-        <v>0.37785999999999997</v>
+        <v>0.37184</v>
       </c>
       <c r="H12" s="369">
         <v>0.54786000000000001</v>
       </c>
-      <c r="J12" s="348" t="e">
+      <c r="J12" s="348" t="b">
         <f>IF(AND(ISNUMBER($E12),ISNUMBER(F12),Trigger),_xll.qlIndexAddFixings(J$3,$E12,F12/100,TRUE),NA())</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K12" s="348" t="e">
+        <v>1</v>
+      </c>
+      <c r="K12" s="348" t="b">
         <f>IF(AND(ISNUMBER($E12),ISNUMBER(G12),Trigger),_xll.qlIndexAddFixings(K$3,$E12,G12/100,TRUE),NA())</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L12" s="348" t="e">
+        <v>1</v>
+      </c>
+      <c r="L12" s="348" t="b">
         <f>IF(AND(ISNUMBER($E12),ISNUMBER(H12),Trigger),_xll.qlIndexAddFixings(L$3,$E12,H12/100,TRUE),NA())</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:190" s="348" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="361">
-        <v>41596</v>
+        <v>41799</v>
       </c>
       <c r="F13" s="362">
-        <v>0.21143000000000001</v>
+        <v>0.20912</v>
       </c>
       <c r="G13" s="362">
-        <v>0.37929000000000002</v>
+        <v>0.37125999999999998</v>
       </c>
       <c r="H13" s="369">
-        <v>0.54903999999999997</v>
-      </c>
-      <c r="J13" s="348" t="e">
+        <v>0.54928999999999994</v>
+      </c>
+      <c r="J13" s="348" t="b">
         <f>IF(AND(ISNUMBER($E13),ISNUMBER(F13),Trigger),_xll.qlIndexAddFixings(J$3,$E13,F13/100,TRUE),NA())</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K13" s="348" t="e">
+        <v>1</v>
+      </c>
+      <c r="K13" s="348" t="b">
         <f>IF(AND(ISNUMBER($E13),ISNUMBER(G13),Trigger),_xll.qlIndexAddFixings(K$3,$E13,G13/100,TRUE),NA())</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L13" s="348" t="e">
+        <v>1</v>
+      </c>
+      <c r="L13" s="348" t="b">
         <f>IF(AND(ISNUMBER($E13),ISNUMBER(H13),Trigger),_xll.qlIndexAddFixings(L$3,$E13,H13/100,TRUE),NA())</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:190" s="348" customFormat="1" x14ac:dyDescent="0.2">
@@ -14173,7 +14166,7 @@
       <c r="U3" s="220"/>
       <c r="V3" s="181">
         <f>_xll.ohTrigger(V5:V23)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W3" s="158"/>
       <c r="X3"/>
@@ -14202,7 +14195,7 @@
       <c r="K4" s="219"/>
       <c r="L4" s="180" t="str">
         <f>_xll.RData(L5:L23,M4:P4,,ReutersRtMode,,M5)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="M4" s="216" t="s">
         <v>160</v>
@@ -15570,7 +15563,7 @@
       <c r="N2" s="182"/>
       <c r="O2" s="181">
         <f>_xll.ohTrigger(O4:O21)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P2" s="158"/>
     </row>
@@ -15595,7 +15588,7 @@
       <c r="H3" s="167"/>
       <c r="I3" s="313" t="str">
         <f>_xll.RData(I4:I21,J3:J3,,ReutersRtMode,,J4)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="J3" s="179" t="s">
         <v>140</v>
@@ -15637,24 +15630,24 @@
         <v>HIHKDOND=</v>
       </c>
       <c r="J4" s="175">
-        <v>5.6610000000000001E-2</v>
+        <v>6.2140000000000001E-2</v>
       </c>
       <c r="K4" s="162" t="s">
         <v>182</v>
       </c>
       <c r="L4" s="174">
-        <v>7.4289999999999995E-2</v>
+        <v>6.2140000000000001E-2</v>
       </c>
       <c r="M4" s="162" t="s">
         <v>182</v>
       </c>
       <c r="N4" s="241">
         <f t="array" ref="N4:N21">QuoteLive</f>
-        <v>5.6610000000000001E-2</v>
+        <v>6.2140000000000001E-2</v>
       </c>
       <c r="O4" s="172">
         <f>_xll.qlSimpleQuoteSetValue(C4,N4/100,ISERROR(D4))</f>
-        <v>0</v>
+        <v>5.5299999999999989E-5</v>
       </c>
       <c r="P4" s="158"/>
     </row>
@@ -15814,23 +15807,23 @@
         <v>HIHKD2WD=</v>
       </c>
       <c r="J8" s="164">
-        <v>0.15643000000000001</v>
+        <v>0.16571</v>
       </c>
       <c r="K8" s="162" t="s">
         <v>182</v>
       </c>
       <c r="L8" s="171">
-        <v>0.15928999999999999</v>
+        <v>0.16571</v>
       </c>
       <c r="M8" s="162" t="s">
         <v>182</v>
       </c>
       <c r="N8" s="230">
-        <v>0.15643000000000001</v>
+        <v>0.16571</v>
       </c>
       <c r="O8" s="168">
         <f>_xll.qlSimpleQuoteSetValue(C8,N8/100,ISERROR(D8))</f>
-        <v>0</v>
+        <v>9.2799999999999654E-5</v>
       </c>
       <c r="P8" s="158"/>
     </row>
@@ -15902,23 +15895,23 @@
         <v>HIHKD1MD=</v>
       </c>
       <c r="J10" s="164">
-        <v>0.20571</v>
+        <v>0.21143000000000001</v>
       </c>
       <c r="K10" s="162" t="s">
         <v>182</v>
       </c>
       <c r="L10" s="171">
-        <v>0.21357000000000001</v>
+        <v>0.21143000000000001</v>
       </c>
       <c r="M10" s="162" t="s">
         <v>182</v>
       </c>
       <c r="N10" s="230">
-        <v>0.20571</v>
+        <v>0.21143000000000001</v>
       </c>
       <c r="O10" s="168">
         <f>_xll.qlSimpleQuoteSetValue(C10,N10/100,ISERROR(D10))</f>
-        <v>0</v>
+        <v>5.7199999999999872E-5</v>
       </c>
       <c r="P10" s="158"/>
     </row>
@@ -15946,23 +15939,23 @@
         <v>HIHKD2MD=</v>
       </c>
       <c r="J11" s="164">
-        <v>0.30286000000000002</v>
+        <v>0.29820000000000002</v>
       </c>
       <c r="K11" s="162" t="s">
         <v>182</v>
       </c>
       <c r="L11" s="171">
-        <v>0.31429000000000001</v>
+        <v>0.29820000000000002</v>
       </c>
       <c r="M11" s="162" t="s">
         <v>182</v>
       </c>
       <c r="N11" s="230">
-        <v>0.30286000000000002</v>
+        <v>0.29820000000000002</v>
       </c>
       <c r="O11" s="168">
         <f>_xll.qlSimpleQuoteSetValue(C11,N11/100,ISERROR(D11))</f>
-        <v>0</v>
+        <v>-4.659999999999994E-5</v>
       </c>
       <c r="P11" s="158"/>
     </row>
@@ -15990,23 +15983,23 @@
         <v>HIHKD3MD=</v>
       </c>
       <c r="J12" s="164">
-        <v>0.37142999999999998</v>
+        <v>0.37357000000000001</v>
       </c>
       <c r="K12" s="162" t="s">
         <v>182</v>
       </c>
       <c r="L12" s="171">
-        <v>0.37857000000000002</v>
+        <v>0.37357000000000001</v>
       </c>
       <c r="M12" s="162" t="s">
         <v>182</v>
       </c>
       <c r="N12" s="230">
-        <v>0.37142999999999998</v>
+        <v>0.37357000000000001</v>
       </c>
       <c r="O12" s="168">
         <f>_xll.qlSimpleQuoteSetValue(C12,N12/100,ISERROR(D12))</f>
-        <v>0</v>
+        <v>2.1400000000000412E-5</v>
       </c>
       <c r="P12" s="158"/>
     </row>
@@ -16033,24 +16026,24 @@
         <f t="shared" si="1"/>
         <v>HIHKD4MD=</v>
       </c>
-      <c r="J13" s="164">
-        <v>0.41356999999999999</v>
+      <c r="J13" s="164" t="s">
+        <v>205</v>
       </c>
       <c r="K13" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="L13" s="171">
-        <v>0.41293000000000002</v>
+      <c r="L13" s="171" t="s">
+        <v>205</v>
       </c>
       <c r="M13" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="N13" s="230">
-        <v>0.41356999999999999</v>
-      </c>
-      <c r="O13" s="168">
+      <c r="N13" s="230" t="str">
+        <v>Record not service permissioned</v>
+      </c>
+      <c r="O13" s="168" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C13,N13/100,ISERROR(D13))</f>
-        <v>9.0000000000003272E-6</v>
+        <v>#NUM!</v>
       </c>
       <c r="P13" s="158"/>
     </row>
@@ -16077,24 +16070,24 @@
         <f t="shared" si="1"/>
         <v>HIHKD5MD=</v>
       </c>
-      <c r="J14" s="164">
-        <v>0.46178999999999998</v>
+      <c r="J14" s="164" t="s">
+        <v>205</v>
       </c>
       <c r="K14" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="L14" s="171">
-        <v>0.46126</v>
+      <c r="L14" s="171" t="s">
+        <v>205</v>
       </c>
       <c r="M14" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="N14" s="230">
-        <v>0.46178999999999998</v>
-      </c>
-      <c r="O14" s="168">
+      <c r="N14" s="230" t="str">
+        <v>Record not service permissioned</v>
+      </c>
+      <c r="O14" s="168" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C14,N14/100,ISERROR(D14))</f>
-        <v>3.599999999999437E-6</v>
+        <v>#NUM!</v>
       </c>
       <c r="P14" s="158"/>
     </row>
@@ -16122,23 +16115,23 @@
         <v>HIHKD6MD=</v>
       </c>
       <c r="J15" s="164">
-        <v>0.54857</v>
+        <v>0.54928999999999994</v>
       </c>
       <c r="K15" s="162" t="s">
         <v>182</v>
       </c>
       <c r="L15" s="171">
-        <v>0.54857</v>
+        <v>0.54928999999999994</v>
       </c>
       <c r="M15" s="162" t="s">
         <v>182</v>
       </c>
       <c r="N15" s="230">
-        <v>0.54857</v>
+        <v>0.54928999999999994</v>
       </c>
       <c r="O15" s="168">
         <f>_xll.qlSimpleQuoteSetValue(C15,N15/100,ISERROR(D15))</f>
-        <v>0</v>
+        <v>7.1999999999997413E-6</v>
       </c>
       <c r="P15" s="158"/>
     </row>
@@ -16165,24 +16158,24 @@
         <f t="shared" si="1"/>
         <v>HIHKD7MD=</v>
       </c>
-      <c r="J16" s="164">
-        <v>0.58213999999999999</v>
+      <c r="J16" s="164" t="s">
+        <v>205</v>
       </c>
       <c r="K16" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="L16" s="171">
-        <v>0.57643</v>
+      <c r="L16" s="171" t="s">
+        <v>205</v>
       </c>
       <c r="M16" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="N16" s="230">
-        <v>0.58213999999999999</v>
-      </c>
-      <c r="O16" s="168">
+      <c r="N16" s="230" t="str">
+        <v>Record not service permissioned</v>
+      </c>
+      <c r="O16" s="168" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C16,N16/100,ISERROR(D16))</f>
-        <v>5.7100000000000033E-5</v>
+        <v>#NUM!</v>
       </c>
       <c r="P16" s="158"/>
     </row>
@@ -16209,24 +16202,24 @@
         <f t="shared" si="1"/>
         <v>HIHKD8MD=</v>
       </c>
-      <c r="J17" s="164">
-        <v>0.61570999999999998</v>
+      <c r="J17" s="164" t="s">
+        <v>205</v>
       </c>
       <c r="K17" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="L17" s="171">
-        <v>0.60958000000000001</v>
+      <c r="L17" s="171" t="s">
+        <v>205</v>
       </c>
       <c r="M17" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="N17" s="230">
-        <v>0.61570999999999998</v>
-      </c>
-      <c r="O17" s="168">
+      <c r="N17" s="230" t="str">
+        <v>Record not service permissioned</v>
+      </c>
+      <c r="O17" s="168" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C17,N17/100,ISERROR(D17))</f>
-        <v>5.4699999999999541E-5</v>
+        <v>#NUM!</v>
       </c>
       <c r="P17" s="158"/>
     </row>
@@ -16253,24 +16246,24 @@
         <f t="shared" si="1"/>
         <v>HIHKD9MD=</v>
       </c>
-      <c r="J18" s="164">
-        <v>0.64856999999999998</v>
+      <c r="J18" s="164" t="s">
+        <v>205</v>
       </c>
       <c r="K18" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="L18" s="171">
-        <v>0.63846999999999998</v>
+      <c r="L18" s="171" t="s">
+        <v>205</v>
       </c>
       <c r="M18" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="N18" s="230">
-        <v>0.64856999999999998</v>
-      </c>
-      <c r="O18" s="168">
+      <c r="N18" s="230" t="str">
+        <v>Record not service permissioned</v>
+      </c>
+      <c r="O18" s="168" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C18,N18/100,ISERROR(D18))</f>
-        <v>9.4299999999999419E-5</v>
+        <v>#NUM!</v>
       </c>
       <c r="P18" s="158"/>
     </row>
@@ -16297,24 +16290,24 @@
         <f t="shared" si="1"/>
         <v>HIHKD10MD=</v>
       </c>
-      <c r="J19" s="164">
-        <v>0.71928999999999998</v>
+      <c r="J19" s="164" t="s">
+        <v>205</v>
       </c>
       <c r="K19" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="L19" s="171">
-        <v>0.71267999999999998</v>
+      <c r="L19" s="171" t="s">
+        <v>205</v>
       </c>
       <c r="M19" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="N19" s="230">
-        <v>0.71928999999999998</v>
-      </c>
-      <c r="O19" s="168">
+      <c r="N19" s="230" t="str">
+        <v>Record not service permissioned</v>
+      </c>
+      <c r="O19" s="168" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C19,N19/100,ISERROR(D19))</f>
-        <v>6.6799999999999672E-5</v>
+        <v>#NUM!</v>
       </c>
       <c r="P19" s="158"/>
     </row>
@@ -16341,24 +16334,24 @@
         <f t="shared" si="1"/>
         <v>HIHKD11MD=</v>
       </c>
-      <c r="J20" s="164">
-        <v>0.79357</v>
+      <c r="J20" s="164" t="s">
+        <v>205</v>
       </c>
       <c r="K20" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="L20" s="171">
-        <v>0.79</v>
+      <c r="L20" s="171" t="s">
+        <v>205</v>
       </c>
       <c r="M20" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="N20" s="230">
-        <v>0.79357</v>
-      </c>
-      <c r="O20" s="168">
+      <c r="N20" s="230" t="str">
+        <v>Record not service permissioned</v>
+      </c>
+      <c r="O20" s="168" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C20,N20/100,ISERROR(D20))</f>
-        <v>4.2799999999999089E-5</v>
+        <v>#NUM!</v>
       </c>
       <c r="P20" s="158"/>
     </row>
@@ -16386,23 +16379,23 @@
         <v>HIHKD1YD=</v>
       </c>
       <c r="J21" s="164">
-        <v>0.86285999999999996</v>
+        <v>0.86356999999999995</v>
       </c>
       <c r="K21" s="162" t="s">
         <v>182</v>
       </c>
       <c r="L21" s="163">
-        <v>0.86570999999999998</v>
+        <v>0.86356999999999995</v>
       </c>
       <c r="M21" s="162" t="s">
         <v>182</v>
       </c>
       <c r="N21" s="223">
-        <v>0.86285999999999996</v>
+        <v>0.86356999999999995</v>
       </c>
       <c r="O21" s="159">
         <f>_xll.qlSimpleQuoteSetValue(C21,N21/100,ISERROR(D21))</f>
-        <v>0</v>
+        <v>7.0999999999994678E-6</v>
       </c>
       <c r="P21" s="158"/>
     </row>
@@ -16545,7 +16538,7 @@
       <c r="V3" s="220"/>
       <c r="W3" s="181">
         <f>_xll.ohTrigger(W7:W28)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X3" s="183"/>
       <c r="Y3" s="190"/>
@@ -16577,7 +16570,7 @@
       <c r="L4" s="217"/>
       <c r="M4" s="180" t="str">
         <f>_xll.RData(M7:M38,N4:Q4,,ReutersRtMode,,N7)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="N4" s="216" t="s">
         <v>160</v>
@@ -16874,10 +16867,10 @@
         <v>HKD1X4F=PREA</v>
       </c>
       <c r="N9" s="212">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="O9" s="212">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="P9" s="211">
         <v>0</v>
@@ -16887,19 +16880,19 @@
       </c>
       <c r="R9" s="175">
         <f>_xll.qlMidSafe($N9,$O9)</f>
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="S9" s="162"/>
       <c r="T9" s="199">
-        <v>0.41000000000000003</v>
+        <v>0.38</v>
       </c>
       <c r="U9" s="162"/>
       <c r="V9" s="230">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="W9" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D9,V9/100,ISERROR(E9))</f>
-        <v>0</v>
+        <v>-2.0000000000000009E-4</v>
       </c>
       <c r="X9" s="158"/>
       <c r="Y9" s="190"/>
@@ -16945,10 +16938,10 @@
         <v>HKD2X5F=PREA</v>
       </c>
       <c r="N10" s="201">
-        <v>0.36</v>
+        <v>0.34</v>
       </c>
       <c r="O10" s="201">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="P10" s="200">
         <v>0</v>
@@ -16958,19 +16951,19 @@
       </c>
       <c r="R10" s="164">
         <f>_xll.qlMidSafe($N10,$O10)</f>
-        <v>0.41000000000000003</v>
+        <v>0.39</v>
       </c>
       <c r="S10" s="162"/>
       <c r="T10" s="199">
-        <v>0.41000000000000003</v>
+        <v>0.39</v>
       </c>
       <c r="U10" s="162"/>
       <c r="V10" s="230">
-        <v>0.41000000000000003</v>
+        <v>0.39</v>
       </c>
       <c r="W10" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D10,V10/100,ISERROR(E10))</f>
-        <v>0</v>
+        <v>-2.0000000000000009E-4</v>
       </c>
       <c r="X10" s="158"/>
       <c r="Y10" s="190"/>
@@ -17016,10 +17009,10 @@
         <v>HKD3X6F=PREA</v>
       </c>
       <c r="N11" s="201">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="O11" s="201">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="P11" s="200">
         <v>0</v>
@@ -17029,19 +17022,19 @@
       </c>
       <c r="R11" s="164">
         <f>_xll.qlMidSafe($N11,$O11)</f>
-        <v>0.41000000000000003</v>
+        <v>0.4</v>
       </c>
       <c r="S11" s="162"/>
       <c r="T11" s="199">
-        <v>0.41000000000000003</v>
+        <v>0.4</v>
       </c>
       <c r="U11" s="162"/>
       <c r="V11" s="230">
-        <v>0.41000000000000003</v>
+        <v>0.4</v>
       </c>
       <c r="W11" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D11,V11/100,ISERROR(E11))</f>
-        <v>0</v>
+        <v>-1.0000000000000026E-4</v>
       </c>
       <c r="X11" s="158"/>
       <c r="Y11" s="190"/>
@@ -17087,10 +17080,10 @@
         <v>HKD4X7F=PREA</v>
       </c>
       <c r="N12" s="201">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="O12" s="201">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="P12" s="200">
         <v>0</v>
@@ -17100,19 +17093,19 @@
       </c>
       <c r="R12" s="164">
         <f>_xll.qlMidSafe($N12,$O12)</f>
-        <v>0.43</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="S12" s="162"/>
       <c r="T12" s="199">
-        <v>0.42</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="U12" s="162"/>
       <c r="V12" s="230">
-        <v>0.43</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="W12" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D12,V12/100,ISERROR(E12))</f>
-        <v>0</v>
+        <v>-1.9999999999999966E-4</v>
       </c>
       <c r="X12" s="158"/>
       <c r="Y12" s="190"/>
@@ -17158,10 +17151,10 @@
         <v>HKD5X8F=PREA</v>
       </c>
       <c r="N13" s="201">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="O13" s="201">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="P13" s="200">
         <v>0</v>
@@ -17171,19 +17164,19 @@
       </c>
       <c r="R13" s="164">
         <f>_xll.qlMidSafe($N13,$O13)</f>
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="S13" s="162"/>
       <c r="T13" s="199">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="U13" s="162"/>
       <c r="V13" s="230">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="W13" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D13,V13/100,ISERROR(E13))</f>
-        <v>0</v>
+        <v>-1.0000000000000026E-4</v>
       </c>
       <c r="X13" s="158"/>
       <c r="Y13" s="190"/>
@@ -17229,10 +17222,10 @@
         <v>HKD6X9F=PREA</v>
       </c>
       <c r="N14" s="201">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="O14" s="201">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="P14" s="200">
         <v>0</v>
@@ -17242,25 +17235,25 @@
       </c>
       <c r="R14" s="164">
         <f>_xll.qlMidSafe($N14,$O14)</f>
-        <v>0.45999999999999996</v>
+        <v>0.44</v>
       </c>
       <c r="S14" s="162"/>
       <c r="T14" s="199">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="U14" s="162"/>
       <c r="V14" s="230">
-        <v>0.45999999999999996</v>
+        <v>0.44</v>
       </c>
       <c r="W14" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D14,V14/100,ISERROR(E14))</f>
-        <v>0</v>
+        <v>-1.9999999999999966E-4</v>
       </c>
       <c r="X14" s="158"/>
       <c r="Y14" s="190"/>
       <c r="Z14" s="191">
         <f t="shared" si="2"/>
-        <v>1.0000000000000009E-3</v>
+        <v>9.999999999999998E-4</v>
       </c>
       <c r="AA14" s="190"/>
     </row>
@@ -17300,10 +17293,10 @@
         <v>HKD7X10F=PREA</v>
       </c>
       <c r="N15" s="201">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="O15" s="201">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="P15" s="200">
         <v>0</v>
@@ -17313,19 +17306,19 @@
       </c>
       <c r="R15" s="164">
         <f>_xll.qlMidSafe($N15,$O15)</f>
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
       <c r="S15" s="162"/>
       <c r="T15" s="199">
-        <v>0.45999999999999996</v>
+        <v>0.47</v>
       </c>
       <c r="U15" s="162"/>
       <c r="V15" s="230">
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
       <c r="W15" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D15,V15/100,ISERROR(E15))</f>
-        <v>0</v>
+        <v>-2.0000000000000052E-4</v>
       </c>
       <c r="X15" s="158"/>
       <c r="Y15" s="190"/>
@@ -17371,10 +17364,10 @@
         <v>HKD8X11F=PREA</v>
       </c>
       <c r="N16" s="201">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="O16" s="201">
-        <v>0.56999999999999995</v>
+        <v>0.54</v>
       </c>
       <c r="P16" s="200">
         <v>0</v>
@@ -17384,25 +17377,25 @@
       </c>
       <c r="R16" s="164">
         <f>_xll.qlMidSafe($N16,$O16)</f>
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
       <c r="S16" s="162"/>
       <c r="T16" s="199">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
       <c r="U16" s="162"/>
       <c r="V16" s="230">
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
       <c r="W16" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D16,V16/100,ISERROR(E16))</f>
-        <v>0</v>
+        <v>-2.9999999999999992E-4</v>
       </c>
       <c r="X16" s="158"/>
       <c r="Y16" s="190"/>
       <c r="Z16" s="191">
         <f t="shared" si="2"/>
-        <v>9.9999999999999872E-4</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="AA16" s="190"/>
     </row>
@@ -17442,10 +17435,10 @@
         <v>HKD9X12F=PREA</v>
       </c>
       <c r="N17" s="207">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="O17" s="207">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P17" s="206">
         <v>0</v>
@@ -17455,19 +17448,19 @@
       </c>
       <c r="R17" s="205">
         <f>_xll.qlMidSafe($N17,$O17)</f>
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="S17" s="162"/>
       <c r="T17" s="204">
-        <v>0.48</v>
+        <v>0.53</v>
       </c>
       <c r="U17" s="162"/>
       <c r="V17" s="230">
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="W17" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D17,V17/100,ISERROR(E17))</f>
-        <v>0</v>
+        <v>-2.0000000000000052E-4</v>
       </c>
       <c r="X17" s="158"/>
       <c r="Y17" s="190"/>
@@ -17657,10 +17650,10 @@
         <v>HKD1X7F=PREA</v>
       </c>
       <c r="N20" s="201">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="O20" s="201">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="P20" s="200">
         <v>0</v>
@@ -17670,19 +17663,19 @@
       </c>
       <c r="R20" s="164">
         <f>_xll.qlMidSafe($N20,$O20)</f>
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="S20" s="162"/>
       <c r="T20" s="199">
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
       <c r="U20" s="162"/>
       <c r="V20" s="230">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="W20" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D20,V20/100,ISERROR(E20))</f>
-        <v>0</v>
+        <v>-1.0000000000000026E-4</v>
       </c>
       <c r="X20" s="158"/>
       <c r="Y20" s="190"/>
@@ -17730,10 +17723,10 @@
         <v>HKD2X8F=PREA</v>
       </c>
       <c r="N21" s="201">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="O21" s="201">
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="P21" s="200">
         <v>0</v>
@@ -17743,19 +17736,19 @@
       </c>
       <c r="R21" s="164">
         <f>_xll.qlMidSafe($N21,$O21)</f>
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="S21" s="162"/>
       <c r="T21" s="199">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="U21" s="162"/>
       <c r="V21" s="230">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="W21" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D21,V21/100,ISERROR(E21))</f>
-        <v>0</v>
+        <v>-2.0000000000000052E-4</v>
       </c>
       <c r="X21" s="158"/>
       <c r="Y21" s="190"/>
@@ -17803,10 +17796,10 @@
         <v>HKD3X9F=PREA</v>
       </c>
       <c r="N22" s="201">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="O22" s="201">
-        <v>0.56000000000000005</v>
+        <v>0.54</v>
       </c>
       <c r="P22" s="200">
         <v>0</v>
@@ -17816,19 +17809,19 @@
       </c>
       <c r="R22" s="164">
         <f>_xll.qlMidSafe($N22,$O22)</f>
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="S22" s="162"/>
       <c r="T22" s="199">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="U22" s="162"/>
       <c r="V22" s="230">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="W22" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D22,V22/100,ISERROR(E22))</f>
-        <v>0</v>
+        <v>-2.0000000000000052E-4</v>
       </c>
       <c r="X22" s="158"/>
       <c r="Y22" s="190"/>
@@ -17876,10 +17869,10 @@
         <v>HKD4X10F=PREA</v>
       </c>
       <c r="N23" s="201">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="O23" s="201">
-        <v>0.57999999999999996</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="P23" s="200">
         <v>0</v>
@@ -17889,7 +17882,7 @@
       </c>
       <c r="R23" s="164">
         <f>_xll.qlMidSafe($N23,$O23)</f>
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
       <c r="S23" s="162"/>
       <c r="T23" s="199">
@@ -17897,17 +17890,17 @@
       </c>
       <c r="U23" s="162"/>
       <c r="V23" s="230">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
       <c r="W23" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D23,V23/100,ISERROR(E23))</f>
-        <v>0</v>
+        <v>-1.9999999999999966E-4</v>
       </c>
       <c r="X23" s="158"/>
       <c r="Y23" s="190"/>
       <c r="Z23" s="191">
         <f t="shared" si="3"/>
-        <v>9.9999999999999872E-4</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="AA23" s="190"/>
     </row>
@@ -17949,10 +17942,10 @@
         <v>HKD5X11F=PREA</v>
       </c>
       <c r="N24" s="201">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="O24" s="201">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P24" s="200">
         <v>0</v>
@@ -17962,19 +17955,19 @@
       </c>
       <c r="R24" s="164">
         <f>_xll.qlMidSafe($N24,$O24)</f>
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="S24" s="162"/>
       <c r="T24" s="199">
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
       <c r="U24" s="162"/>
       <c r="V24" s="230">
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="W24" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D24,V24/100,ISERROR(E24))</f>
-        <v>0</v>
+        <v>-2.0000000000000052E-4</v>
       </c>
       <c r="X24" s="158"/>
       <c r="Y24" s="190"/>
@@ -18022,10 +18015,10 @@
         <v>HKD6X12F=PREA</v>
       </c>
       <c r="N25" s="201">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
       <c r="O25" s="201">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="P25" s="200">
         <v>0</v>
@@ -18035,19 +18028,19 @@
       </c>
       <c r="R25" s="164">
         <f>_xll.qlMidSafe($N25,$O25)</f>
-        <v>0.58000000000000007</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="S25" s="162"/>
       <c r="T25" s="199">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="U25" s="162"/>
       <c r="V25" s="230">
-        <v>0.58000000000000007</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="W25" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D25,V25/100,ISERROR(E25))</f>
-        <v>0</v>
+        <v>-1.9999999999999966E-4</v>
       </c>
       <c r="X25" s="158"/>
       <c r="Y25" s="190"/>
@@ -18460,10 +18453,10 @@
         <v>HKD12X18F=PREA</v>
       </c>
       <c r="N31" s="201">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="O31" s="201">
-        <v>0.93</v>
+        <v>0.99</v>
       </c>
       <c r="P31" s="200">
         <v>0</v>
@@ -18473,19 +18466,19 @@
       </c>
       <c r="R31" s="164">
         <f>_xll.qlMidSafe($N31,$O31)</f>
-        <v>0.88</v>
+        <v>0.94</v>
       </c>
       <c r="S31" s="162"/>
       <c r="T31" s="199">
-        <v>0.6100000000000001</v>
+        <v>0.94</v>
       </c>
       <c r="U31" s="162"/>
       <c r="V31" s="230">
-        <v>0.88</v>
+        <v>0.94</v>
       </c>
       <c r="W31" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D31,V31/100,ISERROR(E31))</f>
-        <v>0</v>
+        <v>5.999999999999981E-4</v>
       </c>
       <c r="X31" s="158"/>
       <c r="Y31" s="190"/>
@@ -18898,10 +18891,10 @@
         <v>HKD18X24F=PREA</v>
       </c>
       <c r="N37" s="201">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="O37" s="201">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="P37" s="200">
         <v>0</v>
@@ -18911,25 +18904,25 @@
       </c>
       <c r="R37" s="164">
         <f>_xll.qlMidSafe($N37,$O37)</f>
-        <v>1.25</v>
+        <v>1.35</v>
       </c>
       <c r="S37" s="162"/>
       <c r="T37" s="199">
-        <v>0.77</v>
+        <v>1.35</v>
       </c>
       <c r="U37" s="162"/>
       <c r="V37" s="230">
-        <v>1.25</v>
+        <v>1.35</v>
       </c>
       <c r="W37" s="168">
         <f>_xll.qlSimpleQuoteSetValue(D37,V37/100,ISERROR(E37))</f>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="X37" s="158"/>
       <c r="Y37" s="190"/>
       <c r="Z37" s="191">
         <f t="shared" si="3"/>
-        <v>1.0000000000000009E-3</v>
+        <v>9.9999999999999655E-4</v>
       </c>
       <c r="AA37" s="190"/>
     </row>
@@ -19510,7 +19503,7 @@
       <c r="Y2" s="220"/>
       <c r="Z2" s="181">
         <f>_xll.ohTrigger(Z4:Z39)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA2" s="247"/>
       <c r="AB2" s="190"/>
@@ -19558,7 +19551,7 @@
       </c>
       <c r="O3" s="254" t="str">
         <f>_xll.RData(O4:O39,P3:T3,,ReutersRtMode,,P4)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:24</v>
       </c>
       <c r="P3" s="251" t="s">
         <v>161</v>
@@ -19606,15 +19599,15 @@
       </c>
       <c r="D4" s="96" t="str">
         <f t="array" ref="D4:D39">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$C4:$C39)</f>
-        <v>J4</v>
+        <v>N4</v>
       </c>
       <c r="E4" s="89" t="str">
         <f t="shared" ref="E4:E35" si="0">Currency&amp;$D$2&amp;$E$2&amp;$D4&amp;QuoteSuffix</f>
-        <v>HKDFUT3MJ4_Quote</v>
+        <v>HKDFUT3MN4_Quote</v>
       </c>
       <c r="F4" s="95" t="str">
         <f>_xll.qlSimpleQuote(E4,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MJ4_Quote#0000</v>
+        <v>HKDFUT3MN4_Quote#0000</v>
       </c>
       <c r="G4" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -19630,53 +19623,53 @@
       </c>
       <c r="M4" s="173" t="str">
         <f t="array" ref="M4:M39">_xll.qlIMMcode(FuturesDates)</f>
-        <v>J4</v>
+        <v>N4</v>
       </c>
       <c r="N4" s="244">
         <f t="array" ref="N4:N39">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,$L4:$L39)</f>
-        <v>41745</v>
+        <v>41836</v>
       </c>
       <c r="O4" s="173" t="str">
         <f>"HIR"&amp;M4</f>
-        <v>HIRJ4</v>
+        <v>HIRN4</v>
       </c>
       <c r="P4" s="243">
-        <v>41743</v>
+        <v>41834</v>
       </c>
       <c r="Q4" s="173">
-        <v>99.54</v>
+        <v>99.55</v>
       </c>
       <c r="R4" s="173">
-        <v>99.64</v>
+        <v>99.65</v>
       </c>
       <c r="S4" s="173">
         <v>0</v>
       </c>
       <c r="T4" s="173">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="U4" s="175">
         <f>_xll.qlMidSafe($Q4,$R4)</f>
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="V4" s="162"/>
       <c r="W4" s="242">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="X4" s="162"/>
       <c r="Y4" s="241">
         <f t="array" ref="Y4:Y39">QuoteLive</f>
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="Z4" s="175">
         <f>_xll.qlSimpleQuoteSetValue(E4,$Y4,ISERROR(F4))</f>
-        <v>0</v>
+        <v>9.9999999999909051E-3</v>
       </c>
       <c r="AA4" s="183"/>
       <c r="AB4" s="190"/>
       <c r="AC4" s="191">
         <f t="shared" ref="AC4:AC39" si="1">(R4-U4)/50</f>
-        <v>9.9999999999994321E-4</v>
+        <v>1.0000000000002273E-3</v>
       </c>
       <c r="AD4" s="190"/>
     </row>
@@ -19689,15 +19682,15 @@
         <v>0</v>
       </c>
       <c r="D5" s="90" t="str">
-        <v>K4</v>
+        <v>Q4</v>
       </c>
       <c r="E5" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MK4_Quote</v>
+        <v>HKDFUT3MQ4_Quote</v>
       </c>
       <c r="F5" s="95" t="str">
         <f>_xll.qlSimpleQuote(E5,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MK4_Quote#0000</v>
+        <v>HKDFUT3MQ4_Quote#0000</v>
       </c>
       <c r="G5" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -19712,51 +19705,51 @@
         <v>0</v>
       </c>
       <c r="M5" s="169" t="str">
-        <v>K4</v>
+        <v>Q4</v>
       </c>
       <c r="N5" s="233">
-        <v>41780</v>
+        <v>41871</v>
       </c>
       <c r="O5" s="169" t="str">
         <f t="shared" ref="O5:O39" si="2">"HIR"&amp;M5</f>
-        <v>HIRK4</v>
+        <v>HIRQ4</v>
       </c>
       <c r="P5" s="232">
-        <v>41778</v>
+        <v>41869</v>
       </c>
       <c r="Q5" s="169">
-        <v>99.54</v>
+        <v>99.55</v>
       </c>
       <c r="R5" s="169">
-        <v>99.64</v>
+        <v>99.65</v>
       </c>
       <c r="S5" s="169">
         <v>0</v>
       </c>
       <c r="T5" s="169">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="U5" s="164">
         <f>_xll.qlMidSafe($Q5,$R5)</f>
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="V5" s="162"/>
       <c r="W5" s="240">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="X5" s="162"/>
       <c r="Y5" s="230">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="Z5" s="164">
         <f>_xll.qlSimpleQuoteSetValue(E5,$Y5,ISERROR(F5))</f>
-        <v>0</v>
+        <v>9.9999999999909051E-3</v>
       </c>
       <c r="AA5" s="183"/>
       <c r="AB5" s="190"/>
       <c r="AC5" s="191">
         <f t="shared" si="1"/>
-        <v>9.9999999999994321E-4</v>
+        <v>1.0000000000002273E-3</v>
       </c>
       <c r="AD5" s="190"/>
     </row>
@@ -19769,15 +19762,15 @@
         <v>0</v>
       </c>
       <c r="D6" s="90" t="str">
-        <v>M4</v>
+        <v>U4</v>
       </c>
       <c r="E6" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MM4_Quote</v>
+        <v>HKDFUT3MU4_Quote</v>
       </c>
       <c r="F6" s="95" t="str">
         <f>_xll.qlSimpleQuote(E6,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MM4_Quote#0000</v>
+        <v>HKDFUT3MU4_Quote#0000</v>
       </c>
       <c r="G6" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -19792,51 +19785,51 @@
         <v>0</v>
       </c>
       <c r="M6" s="169" t="str">
-        <v>M4</v>
+        <v>U4</v>
       </c>
       <c r="N6" s="233">
-        <v>41808</v>
+        <v>41899</v>
       </c>
       <c r="O6" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRM4</v>
+        <v>HIRU4</v>
       </c>
       <c r="P6" s="232">
-        <v>41806</v>
+        <v>41897</v>
       </c>
       <c r="Q6" s="169">
-        <v>99.54</v>
+        <v>99.55</v>
       </c>
       <c r="R6" s="169">
-        <v>99.64</v>
+        <v>99.65</v>
       </c>
       <c r="S6" s="169">
         <v>0</v>
       </c>
       <c r="T6" s="169">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="U6" s="164">
         <f>_xll.qlMidSafe($Q6,$R6)</f>
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="V6" s="162"/>
       <c r="W6" s="240">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="X6" s="162"/>
       <c r="Y6" s="230">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
       <c r="Z6" s="164">
         <f>_xll.qlSimpleQuoteSetValue(E6,$Y6,ISERROR(F6))</f>
-        <v>0</v>
+        <v>9.9999999999909051E-3</v>
       </c>
       <c r="AA6" s="183"/>
       <c r="AB6" s="190"/>
       <c r="AC6" s="191">
         <f t="shared" si="1"/>
-        <v>9.9999999999994321E-4</v>
+        <v>1.0000000000002273E-3</v>
       </c>
       <c r="AD6" s="190"/>
     </row>
@@ -19849,15 +19842,15 @@
         <v>0</v>
       </c>
       <c r="D7" s="90" t="str">
-        <v>N4</v>
+        <v>V4</v>
       </c>
       <c r="E7" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MN4_Quote</v>
+        <v>HKDFUT3MV4_Quote</v>
       </c>
       <c r="F7" s="95" t="str">
         <f>_xll.qlSimpleQuote(E7,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MN4_Quote#0000</v>
+        <v>HKDFUT3MV4_Quote#0000</v>
       </c>
       <c r="G7" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -19872,14 +19865,14 @@
         <v>0</v>
       </c>
       <c r="M7" s="169" t="str">
-        <v>N4</v>
+        <v>V4</v>
       </c>
       <c r="N7" s="233">
-        <v>41836</v>
+        <v>41927</v>
       </c>
       <c r="O7" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRN4</v>
+        <v>HIRV4</v>
       </c>
       <c r="P7" s="232" t="s">
         <v>189</v>
@@ -19901,8 +19894,8 @@
         <v>#NUM!</v>
       </c>
       <c r="V7" s="162"/>
-      <c r="W7" s="240">
-        <v>99.58</v>
+      <c r="W7" s="240" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X7" s="162"/>
       <c r="Y7" s="230" t="e">
@@ -19929,15 +19922,15 @@
         <v>0</v>
       </c>
       <c r="D8" s="90" t="str">
-        <v>Q4</v>
+        <v>X4</v>
       </c>
       <c r="E8" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MQ4_Quote</v>
+        <v>HKDFUT3MX4_Quote</v>
       </c>
       <c r="F8" s="95" t="str">
         <f>_xll.qlSimpleQuote(E8,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MQ4_Quote#0000</v>
+        <v>HKDFUT3MX4_Quote#0000</v>
       </c>
       <c r="G8" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -19952,14 +19945,14 @@
         <v>0</v>
       </c>
       <c r="M8" s="169" t="str">
-        <v>Q4</v>
+        <v>X4</v>
       </c>
       <c r="N8" s="233">
-        <v>41871</v>
+        <v>41962</v>
       </c>
       <c r="O8" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRQ4</v>
+        <v>HIRX4</v>
       </c>
       <c r="P8" s="232" t="s">
         <v>189</v>
@@ -20009,15 +20002,15 @@
         <v>0</v>
       </c>
       <c r="D9" s="90" t="str">
-        <v>U4</v>
+        <v>Z4</v>
       </c>
       <c r="E9" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MU4_Quote</v>
+        <v>HKDFUT3MZ4_Quote</v>
       </c>
       <c r="F9" s="95" t="str">
         <f>_xll.qlSimpleQuote(E9,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MU4_Quote#0000</v>
+        <v>HKDFUT3MZ4_Quote#0000</v>
       </c>
       <c r="G9" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -20032,51 +20025,51 @@
         <v>0</v>
       </c>
       <c r="M9" s="169" t="str">
-        <v>U4</v>
+        <v>Z4</v>
       </c>
       <c r="N9" s="233">
-        <v>41899</v>
+        <v>41990</v>
       </c>
       <c r="O9" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRU4</v>
+        <v>HIRZ4</v>
       </c>
       <c r="P9" s="232">
-        <v>41897</v>
+        <v>41988</v>
       </c>
       <c r="Q9" s="169">
-        <v>99.49</v>
+        <v>99.52</v>
       </c>
       <c r="R9" s="169">
-        <v>99.59</v>
+        <v>99.61</v>
       </c>
       <c r="S9" s="169">
         <v>0</v>
       </c>
       <c r="T9" s="169">
-        <v>99.54</v>
+        <v>99.56</v>
       </c>
       <c r="U9" s="164">
         <f>_xll.qlMidSafe($Q9,$R9)</f>
-        <v>99.539999999999992</v>
+        <v>99.564999999999998</v>
       </c>
       <c r="V9" s="162"/>
-      <c r="W9" s="231" t="e">
-        <v>#NUM!</v>
+      <c r="W9" s="231">
+        <v>99.564999999999998</v>
       </c>
       <c r="X9" s="162"/>
       <c r="Y9" s="230">
-        <v>99.539999999999992</v>
-      </c>
-      <c r="Z9" s="164" t="e">
+        <v>99.564999999999998</v>
+      </c>
+      <c r="Z9" s="164">
         <f>_xll.qlSimpleQuoteSetValue(E9,$Y9,ISERROR(F9))</f>
-        <v>#N/A</v>
+        <v>2.5000000000005684E-2</v>
       </c>
       <c r="AA9" s="183"/>
       <c r="AB9" s="190"/>
       <c r="AC9" s="191">
         <f t="shared" si="1"/>
-        <v>1.0000000000002273E-3</v>
+        <v>9.0000000000003413E-4</v>
       </c>
       <c r="AD9" s="190"/>
     </row>
@@ -20089,15 +20082,15 @@
         <v>0</v>
       </c>
       <c r="D10" s="90" t="str">
-        <v>V4</v>
+        <v>F5</v>
       </c>
       <c r="E10" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MV4_Quote</v>
+        <v>HKDFUT3MF5_Quote</v>
       </c>
       <c r="F10" s="95" t="str">
         <f>_xll.qlSimpleQuote(E10,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MV4_Quote#0000</v>
+        <v>HKDFUT3MF5_Quote#0000</v>
       </c>
       <c r="G10" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -20112,14 +20105,14 @@
         <v>0</v>
       </c>
       <c r="M10" s="169" t="str">
-        <v>V4</v>
+        <v>F5</v>
       </c>
       <c r="N10" s="233">
-        <v>41927</v>
+        <v>42025</v>
       </c>
       <c r="O10" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRV4</v>
+        <v>HIRF5</v>
       </c>
       <c r="P10" s="232" t="s">
         <v>189</v>
@@ -20141,8 +20134,8 @@
         <v>#NUM!</v>
       </c>
       <c r="V10" s="162"/>
-      <c r="W10" s="231">
-        <v>99.539999999999992</v>
+      <c r="W10" s="231" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X10" s="162"/>
       <c r="Y10" s="230" t="e">
@@ -20169,15 +20162,15 @@
         <v>0</v>
       </c>
       <c r="D11" s="90" t="str">
-        <v>X4</v>
+        <v>G5</v>
       </c>
       <c r="E11" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MX4_Quote</v>
+        <v>HKDFUT3MG5_Quote</v>
       </c>
       <c r="F11" s="95" t="str">
         <f>_xll.qlSimpleQuote(E11,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MX4_Quote#0000</v>
+        <v>HKDFUT3MG5_Quote#0000</v>
       </c>
       <c r="G11" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -20192,14 +20185,14 @@
         <v>0</v>
       </c>
       <c r="M11" s="169" t="str">
-        <v>X4</v>
+        <v>G5</v>
       </c>
       <c r="N11" s="233">
-        <v>41962</v>
+        <v>42053</v>
       </c>
       <c r="O11" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRX4</v>
+        <v>HIRG5</v>
       </c>
       <c r="P11" s="232" t="s">
         <v>189</v>
@@ -20249,15 +20242,15 @@
         <v>0</v>
       </c>
       <c r="D12" s="90" t="str">
-        <v>Z4</v>
+        <v>H5</v>
       </c>
       <c r="E12" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MZ4_Quote</v>
+        <v>HKDFUT3MH5_Quote</v>
       </c>
       <c r="F12" s="95" t="str">
         <f>_xll.qlSimpleQuote(E12,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MZ4_Quote#0000</v>
+        <v>HKDFUT3MH5_Quote#0000</v>
       </c>
       <c r="G12" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -20272,51 +20265,51 @@
         <v>0</v>
       </c>
       <c r="M12" s="169" t="str">
-        <v>Z4</v>
+        <v>H5</v>
       </c>
       <c r="N12" s="233">
-        <v>41990</v>
+        <v>42081</v>
       </c>
       <c r="O12" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRZ4</v>
+        <v>HIRH5</v>
       </c>
       <c r="P12" s="232">
-        <v>41988</v>
+        <v>42079</v>
       </c>
       <c r="Q12" s="169">
-        <v>99.42</v>
+        <v>99.43</v>
       </c>
       <c r="R12" s="169">
-        <v>99.52</v>
+        <v>99.5</v>
       </c>
       <c r="S12" s="169">
         <v>0</v>
       </c>
       <c r="T12" s="169">
-        <v>99.46</v>
+        <v>99.45</v>
       </c>
       <c r="U12" s="164">
         <f>_xll.qlMidSafe($Q12,$R12)</f>
-        <v>99.47</v>
+        <v>99.465000000000003</v>
       </c>
       <c r="V12" s="162"/>
-      <c r="W12" s="231" t="e">
-        <v>#NUM!</v>
+      <c r="W12" s="231">
+        <v>99.465000000000003</v>
       </c>
       <c r="X12" s="162"/>
       <c r="Y12" s="230">
-        <v>99.47</v>
-      </c>
-      <c r="Z12" s="164" t="e">
+        <v>99.465000000000003</v>
+      </c>
+      <c r="Z12" s="164">
         <f>_xll.qlSimpleQuoteSetValue(E12,$Y12,ISERROR(F12))</f>
-        <v>#N/A</v>
+        <v>-4.9999999999954525E-3</v>
       </c>
       <c r="AA12" s="183"/>
       <c r="AB12" s="190"/>
       <c r="AC12" s="191">
         <f t="shared" si="1"/>
-        <v>9.9999999999994321E-4</v>
+        <v>6.999999999999318E-4</v>
       </c>
       <c r="AD12" s="190"/>
     </row>
@@ -20329,15 +20322,15 @@
         <v>0</v>
       </c>
       <c r="D13" s="90" t="str">
-        <v>F5</v>
+        <v>J5</v>
       </c>
       <c r="E13" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MF5_Quote</v>
+        <v>HKDFUT3MJ5_Quote</v>
       </c>
       <c r="F13" s="95" t="str">
         <f>_xll.qlSimpleQuote(E13,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MF5_Quote#0000</v>
+        <v>HKDFUT3MJ5_Quote#0000</v>
       </c>
       <c r="G13" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -20352,14 +20345,14 @@
         <v>0</v>
       </c>
       <c r="M13" s="169" t="str">
-        <v>F5</v>
+        <v>J5</v>
       </c>
       <c r="N13" s="233">
-        <v>42025</v>
+        <v>42109</v>
       </c>
       <c r="O13" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRF5</v>
+        <v>HIRJ5</v>
       </c>
       <c r="P13" s="232" t="s">
         <v>189</v>
@@ -20381,8 +20374,8 @@
         <v>#NUM!</v>
       </c>
       <c r="V13" s="162"/>
-      <c r="W13" s="231">
-        <v>99.509999999999991</v>
+      <c r="W13" s="231" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X13" s="162"/>
       <c r="Y13" s="230" t="e">
@@ -20409,15 +20402,15 @@
         <v>0</v>
       </c>
       <c r="D14" s="90" t="str">
-        <v>G5</v>
+        <v>K5</v>
       </c>
       <c r="E14" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MG5_Quote</v>
+        <v>HKDFUT3MK5_Quote</v>
       </c>
       <c r="F14" s="95" t="str">
         <f>_xll.qlSimpleQuote(E14,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MG5_Quote#0000</v>
+        <v>HKDFUT3MK5_Quote#0000</v>
       </c>
       <c r="G14" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -20432,14 +20425,14 @@
         <v>0</v>
       </c>
       <c r="M14" s="169" t="str">
-        <v>G5</v>
+        <v>K5</v>
       </c>
       <c r="N14" s="233">
-        <v>42053</v>
+        <v>42144</v>
       </c>
       <c r="O14" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRG5</v>
+        <v>HIRK5</v>
       </c>
       <c r="P14" s="232" t="s">
         <v>189</v>
@@ -20489,15 +20482,15 @@
         <v>0</v>
       </c>
       <c r="D15" s="90" t="str">
-        <v>H5</v>
+        <v>M5</v>
       </c>
       <c r="E15" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MH5_Quote</v>
+        <v>HKDFUT3MM5_Quote</v>
       </c>
       <c r="F15" s="88" t="str">
         <f>_xll.qlSimpleQuote(E15,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MH5_Quote#0000</v>
+        <v>HKDFUT3MM5_Quote#0000</v>
       </c>
       <c r="G15" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -20512,51 +20505,51 @@
         <v>0</v>
       </c>
       <c r="M15" s="169" t="str">
-        <v>H5</v>
+        <v>M5</v>
       </c>
       <c r="N15" s="233">
-        <v>42081</v>
+        <v>42172</v>
       </c>
       <c r="O15" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRH5</v>
+        <v>HIRM5</v>
       </c>
       <c r="P15" s="232">
-        <v>42079</v>
+        <v>42170</v>
       </c>
       <c r="Q15" s="169">
+        <v>99.23</v>
+      </c>
+      <c r="R15" s="169">
         <v>99.32</v>
       </c>
-      <c r="R15" s="169">
-        <v>99.42</v>
-      </c>
       <c r="S15" s="169">
-        <v>0</v>
+        <v>99.32</v>
       </c>
       <c r="T15" s="169">
-        <v>99.36</v>
+        <v>99.26</v>
       </c>
       <c r="U15" s="164">
         <f>_xll.qlMidSafe($Q15,$R15)</f>
-        <v>99.37</v>
+        <v>99.275000000000006</v>
       </c>
       <c r="V15" s="162"/>
-      <c r="W15" s="231" t="e">
-        <v>#NUM!</v>
+      <c r="W15" s="231">
+        <v>99.275000000000006</v>
       </c>
       <c r="X15" s="162"/>
       <c r="Y15" s="230">
-        <v>99.37</v>
-      </c>
-      <c r="Z15" s="164" t="e">
+        <v>99.275000000000006</v>
+      </c>
+      <c r="Z15" s="164">
         <f>_xll.qlSimpleQuoteSetValue(E15,$Y15,ISERROR(F15))</f>
-        <v>#N/A</v>
+        <v>-9.4999999999998863E-2</v>
       </c>
       <c r="AA15" s="183"/>
       <c r="AB15" s="190"/>
       <c r="AC15" s="191">
         <f t="shared" si="1"/>
-        <v>9.9999999999994321E-4</v>
+        <v>8.9999999999974985E-4</v>
       </c>
       <c r="AD15" s="190"/>
     </row>
@@ -20569,15 +20562,15 @@
         <v>0</v>
       </c>
       <c r="D16" s="90" t="str">
-        <v>J5</v>
+        <v>N5</v>
       </c>
       <c r="E16" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MJ5_Quote</v>
+        <v>HKDFUT3MN5_Quote</v>
       </c>
       <c r="F16" s="88" t="str">
         <f>_xll.qlSimpleQuote(E16,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MJ5_Quote#0000</v>
+        <v>HKDFUT3MN5_Quote#0000</v>
       </c>
       <c r="G16" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -20592,14 +20585,14 @@
         <v>0</v>
       </c>
       <c r="M16" s="169" t="str">
-        <v>J5</v>
+        <v>N5</v>
       </c>
       <c r="N16" s="233">
-        <v>42109</v>
+        <v>42200</v>
       </c>
       <c r="O16" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRJ5</v>
+        <v>HIRN5</v>
       </c>
       <c r="P16" s="232" t="s">
         <v>189</v>
@@ -20649,15 +20642,15 @@
         <v>0</v>
       </c>
       <c r="D17" s="90" t="str">
-        <v>K5</v>
+        <v>Q5</v>
       </c>
       <c r="E17" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MK5_Quote</v>
+        <v>HKDFUT3MQ5_Quote</v>
       </c>
       <c r="F17" s="88" t="str">
         <f>_xll.qlSimpleQuote(E17,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MK5_Quote#0000</v>
+        <v>HKDFUT3MQ5_Quote#0000</v>
       </c>
       <c r="G17" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -20672,14 +20665,14 @@
         <v>0</v>
       </c>
       <c r="M17" s="169" t="str">
-        <v>K5</v>
+        <v>Q5</v>
       </c>
       <c r="N17" s="233">
-        <v>42144</v>
+        <v>42235</v>
       </c>
       <c r="O17" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRK5</v>
+        <v>HIRQ5</v>
       </c>
       <c r="P17" s="232" t="s">
         <v>189</v>
@@ -20729,15 +20722,15 @@
         <v>0</v>
       </c>
       <c r="D18" s="90" t="str">
-        <v>M5</v>
+        <v>U5</v>
       </c>
       <c r="E18" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MM5_Quote</v>
+        <v>HKDFUT3MU5_Quote</v>
       </c>
       <c r="F18" s="88" t="str">
         <f>_xll.qlSimpleQuote(E18,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MM5_Quote#0000</v>
+        <v>HKDFUT3MU5_Quote#0000</v>
       </c>
       <c r="G18" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F18)</f>
@@ -20752,17 +20745,17 @@
         <v>0</v>
       </c>
       <c r="M18" s="169" t="str">
-        <v>M5</v>
+        <v>U5</v>
       </c>
       <c r="N18" s="233">
-        <v>42172</v>
+        <v>42263</v>
       </c>
       <c r="O18" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRM5</v>
+        <v>HIRU5</v>
       </c>
       <c r="P18" s="232">
-        <v>42170</v>
+        <v>42261</v>
       </c>
       <c r="Q18" s="169">
         <v>0</v>
@@ -20774,7 +20767,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="169">
-        <v>99.36</v>
+        <v>99.26</v>
       </c>
       <c r="U18" s="164" t="e">
         <f>_xll.qlMidSafe($Q18,$R18)</f>
@@ -20809,15 +20802,15 @@
         <v>0</v>
       </c>
       <c r="D19" s="90" t="str">
-        <v>N5</v>
+        <v>V5</v>
       </c>
       <c r="E19" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MN5_Quote</v>
+        <v>HKDFUT3MV5_Quote</v>
       </c>
       <c r="F19" s="88" t="str">
         <f>_xll.qlSimpleQuote(E19,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MN5_Quote#0000</v>
+        <v>HKDFUT3MV5_Quote#0000</v>
       </c>
       <c r="G19" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F19)</f>
@@ -20832,14 +20825,14 @@
         <v>0</v>
       </c>
       <c r="M19" s="169" t="str">
-        <v>N5</v>
+        <v>V5</v>
       </c>
       <c r="N19" s="233">
-        <v>42200</v>
+        <v>42298</v>
       </c>
       <c r="O19" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRN5</v>
+        <v>HIRV5</v>
       </c>
       <c r="P19" s="232" t="s">
         <v>189</v>
@@ -20889,15 +20882,15 @@
         <v>0</v>
       </c>
       <c r="D20" s="90" t="str">
-        <v>Q5</v>
+        <v>X5</v>
       </c>
       <c r="E20" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MQ5_Quote</v>
+        <v>HKDFUT3MX5_Quote</v>
       </c>
       <c r="F20" s="88" t="str">
         <f>_xll.qlSimpleQuote(E20,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MQ5_Quote#0000</v>
+        <v>HKDFUT3MX5_Quote#0000</v>
       </c>
       <c r="G20" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F20)</f>
@@ -20912,14 +20905,14 @@
         <v>0</v>
       </c>
       <c r="M20" s="169" t="str">
-        <v>Q5</v>
+        <v>X5</v>
       </c>
       <c r="N20" s="233">
-        <v>42235</v>
+        <v>42326</v>
       </c>
       <c r="O20" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRQ5</v>
+        <v>HIRX5</v>
       </c>
       <c r="P20" s="232" t="s">
         <v>189</v>
@@ -20969,15 +20962,15 @@
         <v>0</v>
       </c>
       <c r="D21" s="90" t="str">
-        <v>U5</v>
+        <v>Z5</v>
       </c>
       <c r="E21" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MU5_Quote</v>
+        <v>HKDFUT3MZ5_Quote</v>
       </c>
       <c r="F21" s="88" t="str">
         <f>_xll.qlSimpleQuote(E21,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MU5_Quote#0000</v>
+        <v>HKDFUT3MZ5_Quote#0000</v>
       </c>
       <c r="G21" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F21)</f>
@@ -20992,17 +20985,17 @@
         <v>0</v>
       </c>
       <c r="M21" s="169" t="str">
-        <v>U5</v>
+        <v>Z5</v>
       </c>
       <c r="N21" s="233">
-        <v>42263</v>
+        <v>42354</v>
       </c>
       <c r="O21" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRU5</v>
+        <v>HIRZ5</v>
       </c>
       <c r="P21" s="232">
-        <v>42261</v>
+        <v>42352</v>
       </c>
       <c r="Q21" s="169">
         <v>0</v>
@@ -21014,7 +21007,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="169">
-        <v>99.36</v>
+        <v>99.26</v>
       </c>
       <c r="U21" s="164" t="e">
         <f>_xll.qlMidSafe($Q21,$R21)</f>
@@ -21049,15 +21042,15 @@
         <v>0</v>
       </c>
       <c r="D22" s="90" t="str">
-        <v>V5</v>
+        <v>F6</v>
       </c>
       <c r="E22" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MV5_Quote</v>
+        <v>HKDFUT3MF6_Quote</v>
       </c>
       <c r="F22" s="88" t="str">
         <f>_xll.qlSimpleQuote(E22,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MV5_Quote#0000</v>
+        <v>HKDFUT3MF6_Quote#0000</v>
       </c>
       <c r="G22" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F22)</f>
@@ -21072,14 +21065,14 @@
         <v>0</v>
       </c>
       <c r="M22" s="169" t="str">
-        <v>V5</v>
+        <v>F6</v>
       </c>
       <c r="N22" s="233">
-        <v>42298</v>
+        <v>42389</v>
       </c>
       <c r="O22" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRV5</v>
+        <v>HIRF6</v>
       </c>
       <c r="P22" s="232" t="s">
         <v>189</v>
@@ -21129,15 +21122,15 @@
         <v>0</v>
       </c>
       <c r="D23" s="90" t="str">
-        <v>X5</v>
+        <v>G6</v>
       </c>
       <c r="E23" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MX5_Quote</v>
+        <v>HKDFUT3MG6_Quote</v>
       </c>
       <c r="F23" s="88" t="str">
         <f>_xll.qlSimpleQuote(E23,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MX5_Quote#0000</v>
+        <v>HKDFUT3MG6_Quote#0000</v>
       </c>
       <c r="G23" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F23)</f>
@@ -21152,14 +21145,14 @@
         <v>0</v>
       </c>
       <c r="M23" s="169" t="str">
-        <v>X5</v>
+        <v>G6</v>
       </c>
       <c r="N23" s="233">
-        <v>42326</v>
+        <v>42417</v>
       </c>
       <c r="O23" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRX5</v>
+        <v>HIRG6</v>
       </c>
       <c r="P23" s="232" t="s">
         <v>189</v>
@@ -21209,15 +21202,15 @@
         <v>0</v>
       </c>
       <c r="D24" s="90" t="str">
-        <v>Z5</v>
+        <v>H6</v>
       </c>
       <c r="E24" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MZ5_Quote</v>
+        <v>HKDFUT3MH6_Quote</v>
       </c>
       <c r="F24" s="88" t="str">
         <f>_xll.qlSimpleQuote(E24,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MZ5_Quote#0000</v>
+        <v>HKDFUT3MH6_Quote#0000</v>
       </c>
       <c r="G24" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F24)</f>
@@ -21232,17 +21225,17 @@
         <v>0</v>
       </c>
       <c r="M24" s="169" t="str">
-        <v>Z5</v>
+        <v>H6</v>
       </c>
       <c r="N24" s="233">
-        <v>42354</v>
+        <v>42445</v>
       </c>
       <c r="O24" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRZ5</v>
+        <v>HIRH6</v>
       </c>
       <c r="P24" s="232">
-        <v>42352</v>
+        <v>42443</v>
       </c>
       <c r="Q24" s="169">
         <v>0</v>
@@ -21254,7 +21247,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="169">
-        <v>99.36</v>
+        <v>99.26</v>
       </c>
       <c r="U24" s="164" t="e">
         <f>_xll.qlMidSafe($Q24,$R24)</f>
@@ -21289,15 +21282,15 @@
         <v>0</v>
       </c>
       <c r="D25" s="90" t="str">
-        <v>F6</v>
+        <v>J6</v>
       </c>
       <c r="E25" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MF6_Quote</v>
+        <v>HKDFUT3MJ6_Quote</v>
       </c>
       <c r="F25" s="88" t="str">
         <f>_xll.qlSimpleQuote(E25,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MF6_Quote#0000</v>
+        <v>HKDFUT3MJ6_Quote#0000</v>
       </c>
       <c r="G25" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F25)</f>
@@ -21312,14 +21305,14 @@
         <v>0</v>
       </c>
       <c r="M25" s="169" t="str">
-        <v>F6</v>
+        <v>J6</v>
       </c>
       <c r="N25" s="233">
-        <v>42389</v>
+        <v>42480</v>
       </c>
       <c r="O25" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRF6</v>
+        <v>HIRJ6</v>
       </c>
       <c r="P25" s="232" t="s">
         <v>189</v>
@@ -21369,15 +21362,15 @@
         <v>0</v>
       </c>
       <c r="D26" s="90" t="str">
-        <v>G6</v>
+        <v>K6</v>
       </c>
       <c r="E26" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MG6_Quote</v>
+        <v>HKDFUT3MK6_Quote</v>
       </c>
       <c r="F26" s="88" t="str">
         <f>_xll.qlSimpleQuote(E26,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MG6_Quote#0000</v>
+        <v>HKDFUT3MK6_Quote#0000</v>
       </c>
       <c r="G26" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F26)</f>
@@ -21392,14 +21385,14 @@
         <v>0</v>
       </c>
       <c r="M26" s="169" t="str">
-        <v>G6</v>
+        <v>K6</v>
       </c>
       <c r="N26" s="233">
-        <v>42417</v>
+        <v>42508</v>
       </c>
       <c r="O26" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRG6</v>
+        <v>HIRK6</v>
       </c>
       <c r="P26" s="232" t="s">
         <v>189</v>
@@ -21449,15 +21442,15 @@
         <v>0</v>
       </c>
       <c r="D27" s="90" t="str">
-        <v>H6</v>
+        <v>M6</v>
       </c>
       <c r="E27" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MH6_Quote</v>
+        <v>HKDFUT3MM6_Quote</v>
       </c>
       <c r="F27" s="88" t="str">
         <f>_xll.qlSimpleQuote(E27,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MH6_Quote#0000</v>
+        <v>HKDFUT3MM6_Quote#0000</v>
       </c>
       <c r="G27" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F27)</f>
@@ -21472,17 +21465,17 @@
         <v>0</v>
       </c>
       <c r="M27" s="169" t="str">
-        <v>H6</v>
+        <v>M6</v>
       </c>
       <c r="N27" s="233">
-        <v>42445</v>
+        <v>42536</v>
       </c>
       <c r="O27" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRH6</v>
+        <v>HIRM6</v>
       </c>
       <c r="P27" s="232">
-        <v>42443</v>
+        <v>42534</v>
       </c>
       <c r="Q27" s="169">
         <v>0</v>
@@ -21494,7 +21487,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="169">
-        <v>99.36</v>
+        <v>99.26</v>
       </c>
       <c r="U27" s="164" t="e">
         <f>_xll.qlMidSafe($Q27,$R27)</f>
@@ -21529,15 +21522,15 @@
         <v>0</v>
       </c>
       <c r="D28" s="90" t="str">
-        <v>J6</v>
+        <v>N6</v>
       </c>
       <c r="E28" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MJ6_Quote</v>
+        <v>HKDFUT3MN6_Quote</v>
       </c>
       <c r="F28" s="88" t="str">
         <f>_xll.qlSimpleQuote(E28,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MJ6_Quote#0000</v>
+        <v>HKDFUT3MN6_Quote#0000</v>
       </c>
       <c r="G28" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F28)</f>
@@ -21552,14 +21545,14 @@
         <v>0</v>
       </c>
       <c r="M28" s="169" t="str">
-        <v>J6</v>
+        <v>N6</v>
       </c>
       <c r="N28" s="233">
-        <v>42480</v>
+        <v>42571</v>
       </c>
       <c r="O28" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRJ6</v>
+        <v>HIRN6</v>
       </c>
       <c r="P28" s="232" t="s">
         <v>189</v>
@@ -21609,15 +21602,15 @@
         <v>0</v>
       </c>
       <c r="D29" s="90" t="str">
-        <v>K6</v>
+        <v>Q6</v>
       </c>
       <c r="E29" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MK6_Quote</v>
+        <v>HKDFUT3MQ6_Quote</v>
       </c>
       <c r="F29" s="88" t="str">
         <f>_xll.qlSimpleQuote(E29,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MK6_Quote#0000</v>
+        <v>HKDFUT3MQ6_Quote#0000</v>
       </c>
       <c r="G29" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F29)</f>
@@ -21632,14 +21625,14 @@
         <v>0</v>
       </c>
       <c r="M29" s="169" t="str">
-        <v>K6</v>
+        <v>Q6</v>
       </c>
       <c r="N29" s="233">
-        <v>42508</v>
+        <v>42599</v>
       </c>
       <c r="O29" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRK6</v>
+        <v>HIRQ6</v>
       </c>
       <c r="P29" s="232" t="s">
         <v>189</v>
@@ -21689,15 +21682,15 @@
         <v>0</v>
       </c>
       <c r="D30" s="90" t="str">
-        <v>M6</v>
+        <v>U6</v>
       </c>
       <c r="E30" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MM6_Quote</v>
+        <v>HKDFUT3MU6_Quote</v>
       </c>
       <c r="F30" s="88" t="str">
         <f>_xll.qlSimpleQuote(E30,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MM6_Quote#0000</v>
+        <v>HKDFUT3MU6_Quote#0000</v>
       </c>
       <c r="G30" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F30)</f>
@@ -21712,14 +21705,14 @@
         <v>0</v>
       </c>
       <c r="M30" s="169" t="str">
-        <v>M6</v>
+        <v>U6</v>
       </c>
       <c r="N30" s="233">
-        <v>42536</v>
+        <v>42634</v>
       </c>
       <c r="O30" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRM6</v>
+        <v>HIRU6</v>
       </c>
       <c r="P30" s="232" t="s">
         <v>189</v>
@@ -21769,15 +21762,15 @@
         <v>0</v>
       </c>
       <c r="D31" s="90" t="str">
-        <v>N6</v>
+        <v>V6</v>
       </c>
       <c r="E31" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MN6_Quote</v>
+        <v>HKDFUT3MV6_Quote</v>
       </c>
       <c r="F31" s="88" t="str">
         <f>_xll.qlSimpleQuote(E31,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MN6_Quote#0000</v>
+        <v>HKDFUT3MV6_Quote#0000</v>
       </c>
       <c r="G31" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F31)</f>
@@ -21792,14 +21785,14 @@
         <v>0</v>
       </c>
       <c r="M31" s="169" t="str">
-        <v>N6</v>
+        <v>V6</v>
       </c>
       <c r="N31" s="233">
-        <v>42571</v>
+        <v>42662</v>
       </c>
       <c r="O31" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRN6</v>
+        <v>HIRV6</v>
       </c>
       <c r="P31" s="232" t="s">
         <v>189</v>
@@ -21849,15 +21842,15 @@
         <v>0</v>
       </c>
       <c r="D32" s="90" t="str">
-        <v>Q6</v>
+        <v>X6</v>
       </c>
       <c r="E32" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MQ6_Quote</v>
+        <v>HKDFUT3MX6_Quote</v>
       </c>
       <c r="F32" s="88" t="str">
         <f>_xll.qlSimpleQuote(E32,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MQ6_Quote#0000</v>
+        <v>HKDFUT3MX6_Quote#0000</v>
       </c>
       <c r="G32" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F32)</f>
@@ -21872,14 +21865,14 @@
         <v>0</v>
       </c>
       <c r="M32" s="169" t="str">
-        <v>Q6</v>
+        <v>X6</v>
       </c>
       <c r="N32" s="233">
-        <v>42599</v>
+        <v>42690</v>
       </c>
       <c r="O32" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRQ6</v>
+        <v>HIRX6</v>
       </c>
       <c r="P32" s="232" t="s">
         <v>189</v>
@@ -21929,15 +21922,15 @@
         <v>0</v>
       </c>
       <c r="D33" s="90" t="str">
-        <v>U6</v>
+        <v>Z6</v>
       </c>
       <c r="E33" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MU6_Quote</v>
+        <v>HKDFUT3MZ6_Quote</v>
       </c>
       <c r="F33" s="88" t="str">
         <f>_xll.qlSimpleQuote(E33,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MU6_Quote#0000</v>
+        <v>HKDFUT3MZ6_Quote#0000</v>
       </c>
       <c r="G33" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F33)</f>
@@ -21952,14 +21945,14 @@
         <v>0</v>
       </c>
       <c r="M33" s="169" t="str">
-        <v>U6</v>
+        <v>Z6</v>
       </c>
       <c r="N33" s="233">
-        <v>42634</v>
+        <v>42725</v>
       </c>
       <c r="O33" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRU6</v>
+        <v>HIRZ6</v>
       </c>
       <c r="P33" s="232" t="s">
         <v>189</v>
@@ -22009,15 +22002,15 @@
         <v>0</v>
       </c>
       <c r="D34" s="90" t="str">
-        <v>V6</v>
+        <v>F7</v>
       </c>
       <c r="E34" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MV6_Quote</v>
+        <v>HKDFUT3MF7_Quote</v>
       </c>
       <c r="F34" s="88" t="str">
         <f>_xll.qlSimpleQuote(E34,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MV6_Quote#0000</v>
+        <v>HKDFUT3MF7_Quote#0000</v>
       </c>
       <c r="G34" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F34)</f>
@@ -22032,14 +22025,14 @@
         <v>0</v>
       </c>
       <c r="M34" s="169" t="str">
-        <v>V6</v>
+        <v>F7</v>
       </c>
       <c r="N34" s="233">
-        <v>42662</v>
+        <v>42753</v>
       </c>
       <c r="O34" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRV6</v>
+        <v>HIRF7</v>
       </c>
       <c r="P34" s="232" t="s">
         <v>189</v>
@@ -22089,15 +22082,15 @@
         <v>0</v>
       </c>
       <c r="D35" s="90" t="str">
-        <v>X6</v>
+        <v>G7</v>
       </c>
       <c r="E35" s="89" t="str">
         <f t="shared" si="0"/>
-        <v>HKDFUT3MX6_Quote</v>
+        <v>HKDFUT3MG7_Quote</v>
       </c>
       <c r="F35" s="88" t="str">
         <f>_xll.qlSimpleQuote(E35,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MX6_Quote#0000</v>
+        <v>HKDFUT3MG7_Quote#0000</v>
       </c>
       <c r="G35" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F35)</f>
@@ -22112,14 +22105,14 @@
         <v>0</v>
       </c>
       <c r="M35" s="169" t="str">
-        <v>X6</v>
+        <v>G7</v>
       </c>
       <c r="N35" s="233">
-        <v>42690</v>
+        <v>42781</v>
       </c>
       <c r="O35" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRX6</v>
+        <v>HIRG7</v>
       </c>
       <c r="P35" s="232" t="s">
         <v>189</v>
@@ -22169,15 +22162,15 @@
         <v>0</v>
       </c>
       <c r="D36" s="90" t="str">
-        <v>Z6</v>
+        <v>H7</v>
       </c>
       <c r="E36" s="89" t="str">
         <f t="shared" ref="E36:E39" si="3">Currency&amp;$D$2&amp;$E$2&amp;$D36&amp;QuoteSuffix</f>
-        <v>HKDFUT3MZ6_Quote</v>
+        <v>HKDFUT3MH7_Quote</v>
       </c>
       <c r="F36" s="88" t="str">
         <f>_xll.qlSimpleQuote(E36,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MZ6_Quote#0000</v>
+        <v>HKDFUT3MH7_Quote#0000</v>
       </c>
       <c r="G36" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F36)</f>
@@ -22192,14 +22185,14 @@
         <v>0</v>
       </c>
       <c r="M36" s="169" t="str">
-        <v>Z6</v>
+        <v>H7</v>
       </c>
       <c r="N36" s="233">
-        <v>42725</v>
+        <v>42809</v>
       </c>
       <c r="O36" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRZ6</v>
+        <v>HIRH7</v>
       </c>
       <c r="P36" s="232" t="s">
         <v>189</v>
@@ -22249,15 +22242,15 @@
         <v>0</v>
       </c>
       <c r="D37" s="90" t="str">
-        <v>F7</v>
+        <v>J7</v>
       </c>
       <c r="E37" s="89" t="str">
         <f t="shared" si="3"/>
-        <v>HKDFUT3MF7_Quote</v>
+        <v>HKDFUT3MJ7_Quote</v>
       </c>
       <c r="F37" s="88" t="str">
         <f>_xll.qlSimpleQuote(E37,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MF7_Quote#0000</v>
+        <v>HKDFUT3MJ7_Quote#0000</v>
       </c>
       <c r="G37" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F37)</f>
@@ -22272,14 +22265,14 @@
         <v>0</v>
       </c>
       <c r="M37" s="169" t="str">
-        <v>F7</v>
+        <v>J7</v>
       </c>
       <c r="N37" s="233">
-        <v>42753</v>
+        <v>42844</v>
       </c>
       <c r="O37" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRF7</v>
+        <v>HIRJ7</v>
       </c>
       <c r="P37" s="232" t="s">
         <v>189</v>
@@ -22329,15 +22322,15 @@
         <v>0</v>
       </c>
       <c r="D38" s="90" t="str">
-        <v>G7</v>
+        <v>K7</v>
       </c>
       <c r="E38" s="89" t="str">
         <f t="shared" si="3"/>
-        <v>HKDFUT3MG7_Quote</v>
+        <v>HKDFUT3MK7_Quote</v>
       </c>
       <c r="F38" s="88" t="str">
         <f>_xll.qlSimpleQuote(E38,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MG7_Quote#0000</v>
+        <v>HKDFUT3MK7_Quote#0000</v>
       </c>
       <c r="G38" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F38)</f>
@@ -22352,14 +22345,14 @@
         <v>0</v>
       </c>
       <c r="M38" s="169" t="str">
-        <v>G7</v>
+        <v>K7</v>
       </c>
       <c r="N38" s="233">
-        <v>42781</v>
+        <v>42872</v>
       </c>
       <c r="O38" s="169" t="str">
         <f t="shared" si="2"/>
-        <v>HIRG7</v>
+        <v>HIRK7</v>
       </c>
       <c r="P38" s="232" t="s">
         <v>189</v>
@@ -22409,15 +22402,15 @@
         <v>0</v>
       </c>
       <c r="D39" s="90" t="str">
-        <v>H7</v>
+        <v>M7</v>
       </c>
       <c r="E39" s="89" t="str">
         <f t="shared" si="3"/>
-        <v>HKDFUT3MH7_Quote</v>
+        <v>HKDFUT3MM7_Quote</v>
       </c>
       <c r="F39" s="88" t="str">
         <f>_xll.qlSimpleQuote(E39,,PriceTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKDFUT3MH7_Quote#0000</v>
+        <v>HKDFUT3MM7_Quote#0000</v>
       </c>
       <c r="G39" s="52" t="str">
         <f>_xll.ohRangeRetrieveError(F39)</f>
@@ -22432,14 +22425,14 @@
         <v>0</v>
       </c>
       <c r="M39" s="160" t="str">
-        <v>H7</v>
+        <v>M7</v>
       </c>
       <c r="N39" s="226">
-        <v>42809</v>
+        <v>42907</v>
       </c>
       <c r="O39" s="160" t="str">
         <f t="shared" si="2"/>
-        <v>HIRH7</v>
+        <v>HIRM7</v>
       </c>
       <c r="P39" s="225" t="s">
         <v>189</v>
@@ -22639,7 +22632,7 @@
       <c r="U3" s="220"/>
       <c r="V3" s="181">
         <f>_xll.ohTrigger(V5:V15)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W3" s="158"/>
       <c r="X3"/>
@@ -22670,7 +22663,7 @@
       <c r="K4" s="219"/>
       <c r="L4" s="180" t="str">
         <f>_xll.RData(L5:L15,M4:P4,,ReutersRtMode,,M5)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="M4" s="216" t="s">
         <v>160</v>
@@ -23012,10 +23005,10 @@
         <v>HKDAM1H6M=PREA</v>
       </c>
       <c r="M9" s="201">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="N9" s="201">
-        <v>0.28999999999999998</v>
+        <v>0.27</v>
       </c>
       <c r="O9" s="201">
         <v>0</v>
@@ -23025,19 +23018,19 @@
       </c>
       <c r="Q9" s="260">
         <f>_xll.qlMidSafe($M9,$N9)</f>
-        <v>0.24</v>
+        <v>0.22000000000000003</v>
       </c>
       <c r="R9" s="162"/>
       <c r="S9" s="171">
-        <v>0.23</v>
+        <v>0.22000000000000003</v>
       </c>
       <c r="T9" s="162"/>
       <c r="U9" s="230">
-        <v>0.24</v>
+        <v>0.22000000000000003</v>
       </c>
       <c r="V9" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E9,U9/100,ISERROR(F9))</f>
-        <v>0</v>
+        <v>-1.9999999999999966E-4</v>
       </c>
       <c r="W9" s="158"/>
       <c r="X9"/>
@@ -23216,10 +23209,10 @@
         <v>HKDAM1H9M=PREA</v>
       </c>
       <c r="M12" s="201">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="N12" s="201">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="O12" s="201">
         <v>0</v>
@@ -23229,19 +23222,19 @@
       </c>
       <c r="Q12" s="260">
         <f>_xll.qlMidSafe($M12,$N12)</f>
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="R12" s="162"/>
       <c r="S12" s="171">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="T12" s="162"/>
       <c r="U12" s="230">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="V12" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E12,U12/100,ISERROR(F12))</f>
-        <v>0</v>
+        <v>-9.9999999999999829E-5</v>
       </c>
       <c r="W12" s="158"/>
       <c r="X12"/>
@@ -23420,10 +23413,10 @@
         <v>HKDAM1H1Y=PREA</v>
       </c>
       <c r="M15" s="207">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="N15" s="207">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
       <c r="O15" s="207">
         <v>0</v>
@@ -23433,19 +23426,19 @@
       </c>
       <c r="Q15" s="258">
         <f>_xll.qlMidSafe($M15,$N15)</f>
-        <v>0.29000000000000004</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R15" s="162"/>
       <c r="S15" s="163">
-        <v>0.29000000000000004</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="T15" s="162"/>
       <c r="U15" s="223">
-        <v>0.29000000000000004</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="V15" s="159">
         <f>_xll.qlSimpleQuoteSetValue(E15,U15/100,ISERROR(F15))</f>
-        <v>0</v>
+        <v>-9.9999999999999829E-5</v>
       </c>
       <c r="W15" s="158"/>
       <c r="X15"/>
@@ -23612,7 +23605,7 @@
       <c r="U3" s="220"/>
       <c r="V3" s="181">
         <f>_xll.ohTrigger(V5:V32)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W3" s="158"/>
       <c r="X3" s="190"/>
@@ -23645,7 +23638,7 @@
       <c r="K4" s="219"/>
       <c r="L4" s="180" t="str">
         <f>_xll.RData(L5:L32,M4:P4,,ReutersRtMode,,M5)</f>
-        <v>Updated at 10:23:59</v>
+        <v>Updated at 09:38:20</v>
       </c>
       <c r="M4" s="216" t="s">
         <v>160</v>
@@ -23714,10 +23707,10 @@
         <v>HKDQM3H6M=PREA</v>
       </c>
       <c r="M5" s="201">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="N5" s="201">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="O5" s="201">
         <v>0</v>
@@ -23727,20 +23720,20 @@
       </c>
       <c r="Q5" s="164">
         <f>_xll.qlMidSafe($M5,$N5)</f>
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="R5" s="162"/>
       <c r="S5" s="171">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="T5" s="162"/>
       <c r="U5" s="230">
         <f t="array" ref="U5:U32">QuoteLive</f>
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="V5" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E5,U5/100,ISERROR(F5))</f>
-        <v>0</v>
+        <v>-2.0000000000000009E-4</v>
       </c>
       <c r="W5" s="158"/>
       <c r="X5" s="190"/>
@@ -23783,10 +23776,10 @@
         <v>HKDQM3H1Y=PREA</v>
       </c>
       <c r="M6" s="201">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="N6" s="201">
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
       <c r="O6" s="201">
         <v>0</v>
@@ -23796,19 +23789,19 @@
       </c>
       <c r="Q6" s="164">
         <f>_xll.qlMidSafe($M6,$N6)</f>
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="R6" s="162"/>
       <c r="S6" s="171">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="T6" s="162"/>
       <c r="U6" s="230">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="V6" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E6,U6/100,ISERROR(F6))</f>
-        <v>0</v>
+        <v>-2.0000000000000052E-4</v>
       </c>
       <c r="W6" s="158"/>
       <c r="X6" s="190"/>
@@ -23919,10 +23912,10 @@
         <v>HKDQM3H18M=PREA</v>
       </c>
       <c r="M8" s="201">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="N8" s="201">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="O8" s="201">
         <v>0</v>
@@ -23932,19 +23925,19 @@
       </c>
       <c r="Q8" s="164">
         <f>_xll.qlMidSafe($M8,$N8)</f>
-        <v>0.55000000000000004</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="R8" s="162"/>
       <c r="S8" s="171">
-        <v>0.45999999999999996</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="T8" s="162"/>
       <c r="U8" s="230">
-        <v>0.55000000000000004</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="V8" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E8,U8/100,ISERROR(F8))</f>
-        <v>0</v>
+        <v>1.9999999999999966E-4</v>
       </c>
       <c r="W8" s="158"/>
       <c r="X8" s="190"/>
@@ -24055,10 +24048,10 @@
         <v>HKDQM3H2Y=PREA</v>
       </c>
       <c r="M10" s="201">
-        <v>0.67</v>
+        <v>0.7</v>
       </c>
       <c r="N10" s="201">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="O10" s="201">
         <v>0</v>
@@ -24068,19 +24061,19 @@
       </c>
       <c r="Q10" s="164">
         <f>_xll.qlMidSafe($M10,$N10)</f>
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
       <c r="R10" s="162"/>
       <c r="S10" s="171">
-        <v>0.53</v>
+        <v>0.75</v>
       </c>
       <c r="T10" s="162"/>
       <c r="U10" s="230">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
       <c r="V10" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E10,U10/100,ISERROR(F10))</f>
-        <v>0</v>
+        <v>2.9999999999999992E-4</v>
       </c>
       <c r="W10" s="158"/>
       <c r="X10" s="190"/>
@@ -24140,7 +24133,7 @@
       </c>
       <c r="R11" s="162"/>
       <c r="S11" s="171">
-        <v>0.76</v>
+        <v>1.17</v>
       </c>
       <c r="T11" s="162"/>
       <c r="U11" s="230">
@@ -24191,10 +24184,10 @@
         <v>HKDQM3H4Y=PREA</v>
       </c>
       <c r="M12" s="201">
-        <v>1.52</v>
+        <v>1.5</v>
       </c>
       <c r="N12" s="201">
-        <v>1.62</v>
+        <v>1.6</v>
       </c>
       <c r="O12" s="201">
         <v>0</v>
@@ -24204,19 +24197,19 @@
       </c>
       <c r="Q12" s="164">
         <f>_xll.qlMidSafe($M12,$N12)</f>
-        <v>1.57</v>
+        <v>1.55</v>
       </c>
       <c r="R12" s="162"/>
       <c r="S12" s="171">
-        <v>1.1200000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="T12" s="162"/>
       <c r="U12" s="230">
-        <v>1.57</v>
+        <v>1.55</v>
       </c>
       <c r="V12" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E12,U12/100,ISERROR(F12))</f>
-        <v>0</v>
+        <v>-2.0000000000000226E-4</v>
       </c>
       <c r="W12" s="158"/>
       <c r="X12" s="190"/>
@@ -24259,10 +24252,10 @@
         <v>HKDQM3H5Y=PREA</v>
       </c>
       <c r="M13" s="201">
-        <v>1.85</v>
+        <v>1.78</v>
       </c>
       <c r="N13" s="201">
-        <v>1.95</v>
+        <v>1.88</v>
       </c>
       <c r="O13" s="201">
         <v>0</v>
@@ -24272,25 +24265,25 @@
       </c>
       <c r="Q13" s="164">
         <f>_xll.qlMidSafe($M13,$N13)</f>
-        <v>1.9</v>
+        <v>1.83</v>
       </c>
       <c r="R13" s="162"/>
       <c r="S13" s="171">
-        <v>1.51</v>
+        <v>1.83</v>
       </c>
       <c r="T13" s="162"/>
       <c r="U13" s="230">
-        <v>1.9</v>
+        <v>1.83</v>
       </c>
       <c r="V13" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E13,U13/100,ISERROR(F13))</f>
-        <v>0</v>
+        <v>-6.9999999999999923E-4</v>
       </c>
       <c r="W13" s="158"/>
       <c r="X13" s="190"/>
       <c r="Y13" s="191">
         <f t="shared" si="2"/>
-        <v>1.0000000000000009E-3</v>
+        <v>9.9999999999999655E-4</v>
       </c>
       <c r="Z13" s="190"/>
     </row>
@@ -24395,10 +24388,10 @@
         <v>HKDQM3H7Y=PREA</v>
       </c>
       <c r="M15" s="201">
-        <v>2.3199999999999998</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="N15" s="201">
-        <v>2.42</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="O15" s="201">
         <v>0</v>
@@ -24408,19 +24401,19 @@
       </c>
       <c r="Q15" s="164">
         <f>_xll.qlMidSafe($M15,$N15)</f>
-        <v>2.37</v>
+        <v>2.23</v>
       </c>
       <c r="R15" s="162"/>
       <c r="S15" s="171">
-        <v>2.0999999999999996</v>
+        <v>2.23</v>
       </c>
       <c r="T15" s="162"/>
       <c r="U15" s="230">
-        <v>2.37</v>
+        <v>2.23</v>
       </c>
       <c r="V15" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E15,U15/100,ISERROR(F15))</f>
-        <v>0</v>
+        <v>-1.4000000000000019E-3</v>
       </c>
       <c r="W15" s="158"/>
       <c r="X15" s="190"/>
@@ -24599,10 +24592,10 @@
         <v>HKDQM3H10Y=PREA</v>
       </c>
       <c r="M18" s="201">
-        <v>2.73</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="N18" s="201">
-        <v>2.83</v>
+        <v>2.63</v>
       </c>
       <c r="O18" s="201">
         <v>0</v>
@@ -24612,19 +24605,19 @@
       </c>
       <c r="Q18" s="164">
         <f>_xll.qlMidSafe($M18,$N18)</f>
-        <v>2.7800000000000002</v>
+        <v>2.58</v>
       </c>
       <c r="R18" s="162"/>
       <c r="S18" s="171">
-        <v>2.63</v>
+        <v>2.58</v>
       </c>
       <c r="T18" s="162"/>
       <c r="U18" s="230">
-        <v>2.7800000000000002</v>
+        <v>2.58</v>
       </c>
       <c r="V18" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E18,U18/100,ISERROR(F18))</f>
-        <v>0</v>
+        <v>-2.0000000000000018E-3</v>
       </c>
       <c r="W18" s="158"/>
       <c r="X18" s="190"/>
@@ -24735,10 +24728,10 @@
         <v>HKDQM3H12Y=PREA</v>
       </c>
       <c r="M20" s="201">
-        <v>2.89</v>
+        <v>2.68</v>
       </c>
       <c r="N20" s="201">
-        <v>2.99</v>
+        <v>2.78</v>
       </c>
       <c r="O20" s="201">
         <v>0</v>
@@ -24748,19 +24741,19 @@
       </c>
       <c r="Q20" s="164">
         <f>_xll.qlMidSafe($M20,$N20)</f>
-        <v>2.9400000000000004</v>
+        <v>2.73</v>
       </c>
       <c r="R20" s="162"/>
       <c r="S20" s="171">
-        <v>2.8200000000000003</v>
+        <v>2.73</v>
       </c>
       <c r="T20" s="162"/>
       <c r="U20" s="230">
-        <v>2.9400000000000004</v>
+        <v>2.73</v>
       </c>
       <c r="V20" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E20,U20/100,ISERROR(F20))</f>
-        <v>0</v>
+        <v>-2.1000000000000012E-3</v>
       </c>
       <c r="W20" s="158"/>
       <c r="X20" s="190"/>
@@ -24939,10 +24932,10 @@
         <v>HKDQM3H15Y=PREA</v>
       </c>
       <c r="M23" s="201">
-        <v>2.97</v>
+        <v>2.79</v>
       </c>
       <c r="N23" s="201">
-        <v>3.07</v>
+        <v>2.89</v>
       </c>
       <c r="O23" s="201">
         <v>0</v>
@@ -24952,25 +24945,25 @@
       </c>
       <c r="Q23" s="164">
         <f>_xll.qlMidSafe($M23,$N23)</f>
-        <v>3.02</v>
+        <v>2.84</v>
       </c>
       <c r="R23" s="162"/>
       <c r="S23" s="171">
-        <v>2.95</v>
+        <v>2.84</v>
       </c>
       <c r="T23" s="162"/>
       <c r="U23" s="230">
-        <v>3.02</v>
+        <v>2.84</v>
       </c>
       <c r="V23" s="168">
         <f>_xll.qlSimpleQuoteSetValue(E23,U23/100,ISERROR(F23))</f>
-        <v>0</v>
+        <v>-1.800000000000003E-3</v>
       </c>
       <c r="W23" s="158"/>
       <c r="X23" s="190"/>
       <c r="Y23" s="191">
         <f t="shared" si="2"/>
-        <v>9.9999999999999655E-4</v>
+        <v>1.0000000000000052E-3</v>
       </c>
       <c r="Z23" s="190"/>
     </row>

</xml_diff>